<commit_message>
More positions and info added
</commit_message>
<xml_diff>
--- a/SVs_identification/results/Summary of monogenous traits.xlsx
+++ b/SVs_identification/results/Summary of monogenous traits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/breedmaps/SVs_identification/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22839A29-1DCA-D44C-9737-63E957142411}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0896A6-3805-3F47-9225-B36257929DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{000CD8DE-5782-4E40-B73D-11CA3F163355}"/>
+    <workbookView xWindow="14140" yWindow="500" windowWidth="14660" windowHeight="16420" xr2:uid="{000CD8DE-5782-4E40-B73D-11CA3F163355}"/>
   </bookViews>
   <sheets>
     <sheet name="All info" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="407">
   <si>
     <r>
       <rPr>
@@ -2401,9 +2401,6 @@
       </rPr>
       <t>Kappa-kasein</t>
     </r>
-  </si>
-  <si>
-    <t>Breed</t>
   </si>
   <si>
     <t>OMIA</t>
@@ -2884,12 +2881,6 @@
     <t>Abortion due to haplotype BH1</t>
   </si>
   <si>
-    <t>BTA7</t>
-  </si>
-  <si>
-    <t>2,811,272 to 47,002,161</t>
-  </si>
-  <si>
     <t>OMIA 001825-9913</t>
   </si>
   <si>
@@ -2960,20 +2951,10 @@
   </si>
   <si>
     <t>Inget ID</t>
-  </si>
-  <si>
-    <t>ENSEMBL SVs</t>
-  </si>
-  <si>
-    <t>ENSEMBL GENOMIC CONTEXT</t>
   </si>
   <si>
     <t>Inget ID
 men kanske denna artikel https://pubmed.ncbi.nlm.nih.gov/27091210/</t>
-  </si>
-  <si>
-    <t>CNV:esv4016828,CNV: esv4011894, CNV:esv4017523,
-INV:esv3896694</t>
   </si>
   <si>
     <t>3 CNVs and 1 INV.
@@ -2999,14 +2980,105 @@
     <t>SNP POS</t>
   </si>
   <si>
-    <t>7?</t>
+    <t>RELEVANCE</t>
+  </si>
+  <si>
+    <t>Causal SNP. Nonsense mutation in FMO3 gene causes fishy milk</t>
+  </si>
+  <si>
+    <t>Causal SNP. Nonsense mutation in SPAST gene</t>
+  </si>
+  <si>
+    <t>All very large CNVs. Comes from studies on beef breeds</t>
+  </si>
+  <si>
+    <t>Likely causal SNP</t>
+  </si>
+  <si>
+    <t>ENSEMBL GENOMIC CONTEXT FOR GENE</t>
+  </si>
+  <si>
+    <t>ENSEMBL SVs IN GENE</t>
+  </si>
+  <si>
+    <t>All large SVs(at least 30 000 000 bp). Comes from studies on dairy cattle</t>
+  </si>
+  <si>
+    <t>ENSEMBL-ID</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000024387</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000021694</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000020597</t>
+  </si>
+  <si>
+    <t>BREED-VEXA</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000007723</t>
+  </si>
+  <si>
+    <t>DEL:esv3894993</t>
+  </si>
+  <si>
+    <t>Small deletion(39 bp). From study on dairy cattle</t>
+  </si>
+  <si>
+    <t>DEL:esv4016828,DEL: esv4011894, DEL:esv4017523,INV:esv3896694</t>
+  </si>
+  <si>
+    <t>DEL:nsv2728340,CNV:nsv2728252</t>
+  </si>
+  <si>
+    <t>CNV:esv4012224,DEL:esv4016814,INV:esv3898433</t>
+  </si>
+  <si>
+    <t>Believed causative SNP but in 2020 italian cattle were found with the phenotype without the mutation</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000019242</t>
+  </si>
+  <si>
+    <t>DEL:nsv2738480,DEL:esv4016522</t>
+  </si>
+  <si>
+    <t>Large CNVs. Comes from studies oon dairy cattle</t>
+  </si>
+  <si>
+    <t>The deletion causes a premature stop codon which terminates 96% of the protein</t>
+  </si>
+  <si>
+    <t>Causal SNP. Nonsense mutation in UBE3B gene</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000018739</t>
+  </si>
+  <si>
+    <t>Likely causal SNP. Splicing variant that has become more and more common</t>
+  </si>
+  <si>
+    <t>DEL:esv4015120,DEL:esv3895598,DEL:esv3895570</t>
+  </si>
+  <si>
+    <t>One small deletion and 2 large CNV.
+Studies on dairy cattle</t>
+  </si>
+  <si>
+    <t>42811272-47002161</t>
+  </si>
+  <si>
+    <t>Lethal haplotype which only exists in Brown Swiss. Somewhere in location 7:42,811,272 to 47,002,161</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3059,12 +3131,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Helvetica"/>
@@ -3077,18 +3143,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF666666"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <u/>
@@ -3108,6 +3162,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF666666"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3187,9 +3253,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3209,18 +3275,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3251,12 +3318,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3803,37 +3891,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53E3D7F1-38C9-AB46-99BA-209E7F03E84D}" name="Tabell1" displayName="Tabell1" ref="A1:AB15" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:AB15" xr:uid="{0AA2673E-FE49-C747-96B4-3C5666F9D2F9}"/>
-  <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{ACE7D78E-E96B-1F4D-8067-F66CD3F7FD27}" name="Breed" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{085AC52D-1D2E-754A-A01E-C239BDEE8C5D}" name="Chr" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{57DD89D0-BA8A-EC41-B6BE-5282B760D848}" name="SNP POS" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{77F86C3C-CF5A-D34D-8A31-6F5D47D6EFA0}" name="GENE START" dataDxfId="1"/>
-    <tableColumn id="28" xr3:uid="{4DA20CC4-1E0E-BB48-932D-5A43187A53BE}" name="GENE END" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{9412F10F-D21D-B546-B7E1-92F91D306254}" name="OMIA" dataDxfId="24"/>
-    <tableColumn id="26" xr3:uid="{15763533-BFA5-604C-9354-4BF9FCB11BAE}" name="ENSEMBL SVs" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{4D5D90D2-809A-DD43-BA84-6410B63686C1}" name="ENSEMBL GENOMIC CONTEXT" dataDxfId="22"/>
-    <tableColumn id="27" xr3:uid="{FD14AF90-18C2-BA4A-A141-A4352E62B16A}" name="VARIANTS FOUND IN DATA" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{8DAC3CF8-AB71-414D-8C5D-72830C12654B}" name="Phenotype" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{58DF4A99-1410-7942-99C6-51B763D195AF}" name="Disease" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{3E2DA18C-B667-C24C-A598-7BD04D408FDE}" name="Species Name" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{B3EE0EC0-4AD8-394E-A5FE-757BE0A69B6C}" name="Breed(s)" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{5ADBCE97-CD44-7842-8957-11E7505F44CF}" name="Variant Phenotype" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{4AD04D23-0239-3946-93C3-1370577299F9}" name="Gene" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{BDF8EFC6-489C-4E4A-9E72-B39B6B4DF80A}" name="Allele" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{49A51C92-58AF-E44D-BD15-32D5D8BADE88}" name="Type of Variant" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{005172F3-431C-1945-A497-EE45DEBF3990}" name="Deleterious?" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{CB932DD3-F260-2240-8C94-7468BF350888}" name="Reference Sequence" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{E41D0773-16F9-204C-89F2-C290FB3E9A4F}" name="Chr." dataDxfId="10"/>
-    <tableColumn id="18" xr3:uid="{33E292B1-706E-9F4C-97DA-DF3FD3139C2C}" name="g. or m." dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{602887C8-31D7-2149-858E-258218F733AA}" name="c. or n." dataDxfId="8"/>
-    <tableColumn id="20" xr3:uid="{EC84F0CA-43F8-FC49-A87F-756544AA4298}" name="p." dataDxfId="7"/>
-    <tableColumn id="21" xr3:uid="{49D440FA-35AB-2F48-A236-10B0AFD7A6BE}" name="Verbal Description" dataDxfId="6"/>
-    <tableColumn id="22" xr3:uid="{FA5B48EE-A951-F64D-A0BE-29507E9E6D79}" name="EVA ID" dataDxfId="5"/>
-    <tableColumn id="23" xr3:uid="{32A953CB-D1BE-0A4A-B305-D3199FBD5323}" name="Year Published" dataDxfId="4"/>
-    <tableColumn id="24" xr3:uid="{7F65A2DA-CDBC-7A49-A7BE-7B31C66C2C9E}" name="PubMed ID(s)" dataDxfId="3"/>
-    <tableColumn id="25" xr3:uid="{62AB2050-AD6B-D045-AA1C-74B4C098A49C}" name="Acknowledgements" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53E3D7F1-38C9-AB46-99BA-209E7F03E84D}" name="Tabell1" displayName="Tabell1" ref="A1:AD15" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A1:AD15" xr:uid="{0AA2673E-FE49-C747-96B4-3C5666F9D2F9}"/>
+  <tableColumns count="30">
+    <tableColumn id="1" xr3:uid="{ACE7D78E-E96B-1F4D-8067-F66CD3F7FD27}" name="BREED-VEXA" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{085AC52D-1D2E-754A-A01E-C239BDEE8C5D}" name="Chr" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{57DD89D0-BA8A-EC41-B6BE-5282B760D848}" name="SNP POS" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{77F86C3C-CF5A-D34D-8A31-6F5D47D6EFA0}" name="GENE START" dataDxfId="25"/>
+    <tableColumn id="28" xr3:uid="{4DA20CC4-1E0E-BB48-932D-5A43187A53BE}" name="GENE END" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{9412F10F-D21D-B546-B7E1-92F91D306254}" name="OMIA" dataDxfId="23"/>
+    <tableColumn id="30" xr3:uid="{EFF9486F-9574-B740-9790-067C818CB30B}" name="ENSEMBL-ID"/>
+    <tableColumn id="26" xr3:uid="{15763533-BFA5-604C-9354-4BF9FCB11BAE}" name="ENSEMBL SVs IN GENE" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{4D5D90D2-809A-DD43-BA84-6410B63686C1}" name="ENSEMBL GENOMIC CONTEXT FOR GENE" dataDxfId="21"/>
+    <tableColumn id="27" xr3:uid="{FD14AF90-18C2-BA4A-A141-A4352E62B16A}" name="VARIANTS FOUND IN DATA" dataDxfId="20"/>
+    <tableColumn id="29" xr3:uid="{0B49611E-A656-1B47-897D-7A419E74B73E}" name="RELEVANCE" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{8DAC3CF8-AB71-414D-8C5D-72830C12654B}" name="Phenotype" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{58DF4A99-1410-7942-99C6-51B763D195AF}" name="Disease" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{3E2DA18C-B667-C24C-A598-7BD04D408FDE}" name="Species Name" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{B3EE0EC0-4AD8-394E-A5FE-757BE0A69B6C}" name="Breed(s)" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{5ADBCE97-CD44-7842-8957-11E7505F44CF}" name="Variant Phenotype" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{4AD04D23-0239-3946-93C3-1370577299F9}" name="Gene" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{BDF8EFC6-489C-4E4A-9E72-B39B6B4DF80A}" name="Allele" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{49A51C92-58AF-E44D-BD15-32D5D8BADE88}" name="Type of Variant" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{005172F3-431C-1945-A497-EE45DEBF3990}" name="Deleterious?" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{CB932DD3-F260-2240-8C94-7468BF350888}" name="Reference Sequence" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{E41D0773-16F9-204C-89F2-C290FB3E9A4F}" name="Chr." dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{33E292B1-706E-9F4C-97DA-DF3FD3139C2C}" name="g. or m." dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{602887C8-31D7-2149-858E-258218F733AA}" name="c. or n." dataDxfId="6"/>
+    <tableColumn id="20" xr3:uid="{EC84F0CA-43F8-FC49-A87F-756544AA4298}" name="p." dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{49D440FA-35AB-2F48-A236-10B0AFD7A6BE}" name="Verbal Description" dataDxfId="4"/>
+    <tableColumn id="22" xr3:uid="{FA5B48EE-A951-F64D-A0BE-29507E9E6D79}" name="EVA ID" dataDxfId="3"/>
+    <tableColumn id="23" xr3:uid="{32A953CB-D1BE-0A4A-B305-D3199FBD5323}" name="Year Published" dataDxfId="2"/>
+    <tableColumn id="24" xr3:uid="{7F65A2DA-CDBC-7A49-A7BE-7B31C66C2C9E}" name="PubMed ID(s)" dataDxfId="1"/>
+    <tableColumn id="25" xr3:uid="{62AB2050-AD6B-D045-AA1C-74B4C098A49C}" name="Acknowledgements" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4136,128 +4226,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5724AFB8-EF24-374C-BA51-A6E5C12EB880}">
-  <dimension ref="A1:AB15"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.1640625" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="62" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="72.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="33" customHeight="1">
+    <row r="1" spans="1:30" ht="33" customHeight="1">
       <c r="A1" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="G1" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="J1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="AB1" s="7" t="s">
-        <v>292</v>
-      </c>
     </row>
-    <row r="2" spans="1:28" ht="51">
+    <row r="2" spans="1:30" s="13" customFormat="1" ht="51">
       <c r="A2" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B2" s="6">
         <v>11</v>
@@ -4265,79 +4364,85 @@
       <c r="C2" s="12">
         <v>14742184</v>
       </c>
-      <c r="D2" t="s">
-        <v>379</v>
-      </c>
-      <c r="E2" t="s">
-        <v>380</v>
+      <c r="D2" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>374</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>375</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="R2" s="6"/>
+      <c r="S2" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="V2" s="6">
+        <v>11</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="T2" s="6">
-        <v>11</v>
-      </c>
-      <c r="U2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6" t="s">
+      <c r="AB2" s="6">
+        <v>2010</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>19714378</v>
+      </c>
+      <c r="AD2" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="Z2" s="6">
-        <v>2010</v>
-      </c>
-      <c r="AA2" s="6">
-        <v>19714378</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>275</v>
-      </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:30" s="13" customFormat="1" ht="17">
       <c r="A3" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B3" s="6">
         <v>16</v>
@@ -4345,71 +4450,85 @@
       <c r="C3" s="6">
         <v>38666821</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="D3" s="6">
+        <v>38649500</v>
+      </c>
+      <c r="E3" s="6">
+        <v>38676494</v>
+      </c>
       <c r="F3" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="M3" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="P3" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="Q3" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="R3" s="6"/>
+      <c r="S3" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="13" t="s">
+      <c r="T3" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="V3" s="15">
+        <v>16</v>
+      </c>
+      <c r="W3" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="R3" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="T3" s="13">
-        <v>16</v>
-      </c>
-      <c r="U3" s="13" t="s">
+      <c r="X3" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="Y3" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="W3" s="13" t="s">
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="13" t="s">
+      <c r="AB3" s="15">
+        <v>2002</v>
+      </c>
+      <c r="AC3" s="15">
+        <v>12466292</v>
+      </c>
+      <c r="AD3" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="Z3" s="13">
-        <v>2002</v>
-      </c>
-      <c r="AA3" s="13">
-        <v>12466292</v>
-      </c>
-      <c r="AB3" s="13" t="s">
-        <v>301</v>
-      </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:30" s="13" customFormat="1">
       <c r="A4" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B4" s="6">
         <v>4</v>
@@ -4417,203 +4536,245 @@
       <c r="C4" s="6">
         <v>49600585</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="M4" s="13" t="s">
+      <c r="D4" s="6">
+        <v>49589564</v>
+      </c>
+      <c r="E4" s="6">
+        <v>49629500</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="P4" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="Q4" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="O4" s="13" t="s">
+      <c r="R4" s="6"/>
+      <c r="S4" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="V4" s="15">
+        <v>4</v>
+      </c>
+      <c r="W4" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="T4" s="13">
-        <v>4</v>
-      </c>
-      <c r="U4" s="13" t="s">
+      <c r="X4" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="V4" s="13" t="s">
+      <c r="Y4" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="W4" s="13" t="s">
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="13" t="s">
+      <c r="AB4" s="15">
+        <v>2016</v>
+      </c>
+      <c r="AC4" s="15">
+        <v>26992691</v>
+      </c>
+      <c r="AD4" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="Z4" s="13">
-        <v>2016</v>
-      </c>
-      <c r="AA4" s="13">
-        <v>26992691</v>
-      </c>
-      <c r="AB4" s="14" t="s">
-        <v>310</v>
-      </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:30" s="13" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B5" s="6">
         <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+        <v>319</v>
+      </c>
+      <c r="D5" s="6">
+        <v>61599658</v>
+      </c>
+      <c r="E5" s="6">
+        <v>61638727</v>
+      </c>
       <c r="F5" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="O5" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="M5" s="13" t="s">
+      <c r="P5" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="Q5" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="R5" s="6"/>
+      <c r="S5" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="T5" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="U5" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="V5" s="15">
+        <v>24</v>
+      </c>
+      <c r="W5" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="T5" s="13">
-        <v>24</v>
-      </c>
-      <c r="U5" s="13" t="s">
+      <c r="X5" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="Y5" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="W5" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="13">
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="15">
         <v>2007</v>
       </c>
-      <c r="AA5" s="13">
+      <c r="AC5" s="15">
         <v>17420465</v>
       </c>
-      <c r="AB5" s="13" t="s">
-        <v>275</v>
+      <c r="AD5" s="15" t="s">
+        <v>274</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:30" s="13" customFormat="1">
       <c r="A6" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B6" s="6">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6" s="6">
+        <v>27116487</v>
+      </c>
+      <c r="E6" s="6">
+        <v>27131137</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>397</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>398</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="O6" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="M6" s="13" t="s">
+      <c r="P6" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="Q6" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="R6" s="6"/>
+      <c r="S6" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="13" t="s">
+      <c r="T6" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="R6" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="13" t="s">
+      <c r="Y6" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="W6" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="13">
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="15">
         <v>2016</v>
       </c>
-      <c r="AA6" s="13">
+      <c r="AC6" s="15">
         <v>27364156</v>
       </c>
-      <c r="AB6" s="6"/>
+      <c r="AD6" s="6"/>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:30" s="13" customFormat="1">
       <c r="A7" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B7" s="6">
         <v>17</v>
@@ -4623,350 +4784,387 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="6" t="s">
+      <c r="F7" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="R7" s="6"/>
+      <c r="S7" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="T7" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="V7" s="15">
+        <v>17</v>
+      </c>
+      <c r="W7" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="AB7" s="15">
+        <v>2014</v>
+      </c>
+      <c r="AC7" s="15">
+        <v>25306138</v>
+      </c>
+      <c r="AD7" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="13" customFormat="1" ht="34">
+      <c r="A8" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>328</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>330</v>
-      </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="R7" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="S7" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="T7" s="13">
-        <v>17</v>
-      </c>
-      <c r="U7" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="V7" s="6"/>
-      <c r="W7" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="Z7" s="13">
-        <v>2014</v>
-      </c>
-      <c r="AA7" s="13">
-        <v>25306138</v>
-      </c>
-      <c r="AB7" s="14" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28">
-      <c r="A8" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="B8" s="6">
         <v>3</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="D8" s="6">
+        <v>50994444</v>
+      </c>
+      <c r="E8" s="6">
+        <v>51122558</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="O8" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="6" t="s">
+      <c r="P8" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q8" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="R8" s="6"/>
+      <c r="S8" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="T8" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="U8" s="6"/>
+      <c r="V8" s="15">
+        <v>3</v>
+      </c>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="15">
+        <v>2017</v>
+      </c>
+      <c r="AC8" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="AD8" s="6"/>
+    </row>
+    <row r="9" spans="1:30" s="13" customFormat="1" ht="34">
+      <c r="A9" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="B9" s="6">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="L8" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="R8" s="13" t="s">
+      <c r="N9" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="P9" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="U9" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="S8" s="6"/>
-      <c r="T8" s="13">
-        <v>3</v>
-      </c>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="13">
-        <v>2017</v>
-      </c>
-      <c r="AA8" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="AB8" s="6"/>
+      <c r="V9" s="6">
+        <v>7</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>2011</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>22118103</v>
+      </c>
+      <c r="AD9" s="6" t="s">
+        <v>311</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" ht="17">
-      <c r="A9" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="6" t="s">
+    <row r="10" spans="1:30" s="13" customFormat="1">
+      <c r="A10" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="U9" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="Z9" s="6">
-        <v>2011</v>
-      </c>
-      <c r="AA9" s="6">
-        <v>22118103</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28">
-      <c r="A10" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="B10" s="6">
         <v>19</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="11">
         <v>10833921</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="N10" s="8" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="R10" s="8"/>
+      <c r="S10" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="U10" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="V10" s="16">
+        <v>19</v>
+      </c>
+      <c r="W10" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="X10" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="Y10" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="R10" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="S10" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="T10" s="8">
-        <v>19</v>
-      </c>
-      <c r="U10" s="8" t="s">
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="V10" s="8" t="s">
+      <c r="AB10" s="16">
+        <v>2016</v>
+      </c>
+      <c r="AC10" s="16">
+        <v>27225349</v>
+      </c>
+      <c r="AD10" s="17" t="s">
         <v>351</v>
       </c>
-      <c r="W10" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="Z10" s="8">
-        <v>2016</v>
-      </c>
-      <c r="AA10" s="8">
-        <v>27225349</v>
-      </c>
-      <c r="AB10" s="10" t="s">
-        <v>354</v>
-      </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:30" s="13" customFormat="1">
       <c r="A11" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="6" t="s">
+      <c r="F11" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q11" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="R11" s="8"/>
+      <c r="S11" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="T11" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="16">
+        <v>2014</v>
+      </c>
+      <c r="AC11" s="16">
+        <v>24391517</v>
+      </c>
+      <c r="AD11" s="8"/>
+    </row>
+    <row r="12" spans="1:30" s="13" customFormat="1" ht="51">
+      <c r="A12" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="R11" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="8">
-        <v>2014</v>
-      </c>
-      <c r="AA11" s="8">
-        <v>24391517</v>
-      </c>
-      <c r="AB11" s="9"/>
-    </row>
-    <row r="12" spans="1:28" ht="51">
-      <c r="A12" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="G12" s="6"/>
+      <c r="F12" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="G12" s="9"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>259</v>
+      </c>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
@@ -4982,101 +5180,105 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:30" s="13" customFormat="1">
       <c r="A13" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B13" s="6">
         <v>13</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="11">
         <v>24024659</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="M13" s="8" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q13" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="R13" s="8"/>
+      <c r="S13" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="T13" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="U13" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="V13" s="16">
+        <v>13</v>
+      </c>
+      <c r="W13" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="X13" s="16" t="s">
         <v>363</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="Y13" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="R13" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="S13" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="T13" s="8">
-        <v>13</v>
-      </c>
-      <c r="U13" s="8" t="s">
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="V13" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="W13" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="Z13" s="8">
+      <c r="AB13" s="16">
         <v>2016</v>
       </c>
-      <c r="AA13" s="8">
+      <c r="AC13" s="16">
         <v>26923438</v>
       </c>
-      <c r="AB13" s="10" t="s">
-        <v>354</v>
+      <c r="AD13" s="17" t="s">
+        <v>351</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:30" s="13" customFormat="1">
       <c r="A14" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>261</v>
+      </c>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -5092,8 +5294,10 @@
       <c r="Z14" s="6"/>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:30">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -5122,19 +5326,20 @@
       <c r="Z15" s="6"/>
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="AB4" r:id="rId1" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{6FB82143-03EF-B943-B3B6-9B4DAEF5B546}"/>
-    <hyperlink ref="AB7" r:id="rId2" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{B60A99FD-0C8B-EC4B-A9FA-00FD4C228C68}"/>
-    <hyperlink ref="AB10" r:id="rId3" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{0F14DC3C-6185-1C4E-9471-581DD7F01AAD}"/>
-    <hyperlink ref="AB13" r:id="rId4" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{10561EFE-5896-9F41-A883-2CDD80893631}"/>
-    <hyperlink ref="D2" r:id="rId5" display="https://www.ensembl.org/Bos_taurus/Location/View?db=core;g=ENSBTAG00000021694;r=11:14696392-14751826" xr:uid="{BF18D42C-7A4A-0340-B8DA-AAEA8B55C310}"/>
+    <hyperlink ref="AD4" r:id="rId1" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{6FB82143-03EF-B943-B3B6-9B4DAEF5B546}"/>
+    <hyperlink ref="AD7" r:id="rId2" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{B60A99FD-0C8B-EC4B-A9FA-00FD4C228C68}"/>
+    <hyperlink ref="AD10" r:id="rId3" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{0F14DC3C-6185-1C4E-9471-581DD7F01AAD}"/>
+    <hyperlink ref="AD13" r:id="rId4" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{10561EFE-5896-9F41-A883-2CDD80893631}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5153,10 +5358,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5173,24 +5378,24 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="24" t="s">
+      <c r="J2" s="26"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="26"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="3" spans="1:13" ht="34">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
Completed checking the monogenous traits
Found SVs that might be connected to Chondrodysplasia
</commit_message>
<xml_diff>
--- a/SVs_identification/results/Summary of monogenous traits.xlsx
+++ b/SVs_identification/results/Summary of monogenous traits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/breedmaps/SVs_identification/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0896A6-3805-3F47-9225-B36257929DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A54BBD-5BA4-B947-B6E2-6D68B2B0BAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14140" yWindow="500" windowWidth="14660" windowHeight="16420" xr2:uid="{000CD8DE-5782-4E40-B73D-11CA3F163355}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{000CD8DE-5782-4E40-B73D-11CA3F163355}"/>
   </bookViews>
   <sheets>
     <sheet name="All info" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="451">
   <si>
     <r>
       <rPr>
@@ -2625,16 +2625,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Chondrodysplasia, recessive (Bulldog)</t>
-    </r>
-  </si>
-  <si>
     <t>OMIA 001247-9913</t>
   </si>
   <si>
@@ -2948,13 +2938,6 @@
   </si>
   <si>
     <t>OMIA 001334-9913</t>
-  </si>
-  <si>
-    <t>Inget ID</t>
-  </si>
-  <si>
-    <t>Inget ID
-men kanske denna artikel https://pubmed.ncbi.nlm.nih.gov/27091210/</t>
   </si>
   <si>
     <t>3 CNVs and 1 INV.
@@ -2971,15 +2954,6 @@
     <t>GENE START</t>
   </si>
   <si>
-    <t>14,696,392</t>
-  </si>
-  <si>
-    <t>14,751,826</t>
-  </si>
-  <si>
-    <t>SNP POS</t>
-  </si>
-  <si>
     <t>RELEVANCE</t>
   </si>
   <si>
@@ -3029,12 +3003,6 @@
   </si>
   <si>
     <t>DEL:esv4016828,DEL: esv4011894, DEL:esv4017523,INV:esv3896694</t>
-  </si>
-  <si>
-    <t>DEL:nsv2728340,CNV:nsv2728252</t>
-  </si>
-  <si>
-    <t>CNV:esv4012224,DEL:esv4016814,INV:esv3898433</t>
   </si>
   <si>
     <t>Believed causative SNP but in 2020 italian cattle were found with the phenotype without the mutation</t>
@@ -3072,6 +3040,192 @@
   </si>
   <si>
     <t>Lethal haplotype which only exists in Brown Swiss. Somewhere in location 7:42,811,272 to 47,002,161</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000002698</t>
+  </si>
+  <si>
+    <t>INV:esv3897355,DEL:esv4016477</t>
+  </si>
+  <si>
+    <t>Large SVs (inv = 46 mil, del = 21 mil bp)
+Studies on dairy cattle</t>
+  </si>
+  <si>
+    <t>DEL:nsv2728480.INV:esv3897455</t>
+  </si>
+  <si>
+    <t>Large SVs(inv= 1mil DEL = 27 mil bp)
+Comes from studies on dairy cattle</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000001290</t>
+  </si>
+  <si>
+    <t>Likely causal SNP. The phenotype and frequency of the mutation has increased in Nordic red dairy cattle</t>
+  </si>
+  <si>
+    <t>SNP/SV POS</t>
+  </si>
+  <si>
+    <t>20100649-20763116</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000020149</t>
+  </si>
+  <si>
+    <t>Some large, some small SVs. One is 600 00 bp long</t>
+  </si>
+  <si>
+    <t>Causal SV. Likely due to the gene RNASEH2B which causes embryonic lethality in mouse in knockout study</t>
+  </si>
+  <si>
+    <t>Stillbirth</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val=".Apple Symbols Fallback"/>
+      </rPr>
+      <t>∼</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>525 KB deletion on Chr23:12,291,761-12,817,087 (overlapping BTBD9, GLO1 and DNAH8)"</t>
+    </r>
+  </si>
+  <si>
+    <t>OMIA 001991-9913</t>
+  </si>
+  <si>
+    <t>12291761-12817087</t>
+  </si>
+  <si>
+    <t>BTBD9, DNAH8, GLO1</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000000529,
+ENSBTAG00000014063,
+ENSBTAG00000012703</t>
+  </si>
+  <si>
+    <t>12062334
+12560570
+12494154</t>
+  </si>
+  <si>
+    <t>12436221
+12888737
+12519916</t>
+  </si>
+  <si>
+    <t>Probable causal SV which includes 3 genes.</t>
+  </si>
+  <si>
+    <t>Some large, some small SVs.
+Comes from both beef and dairy cattle</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000020929</t>
+  </si>
+  <si>
+    <t>DEL:esv4018774</t>
+  </si>
+  <si>
+    <t>BTBD9 - INV:esv3897810,DUP:esv3899664,INV:esv3897812,DUP:esv3899636,DEL:esv4019342
+DNAH8 - INV:esv3897810, DUP:esv3899664,INV:esv3897812,DUP:esv3899636,DEL:esv4019342,DEL:nsv2727244,DEL:esv4014169
+GLO1 - INV:esv3897810,DUP:esv3899664,INV:esv3897812,DUP:esv3899636,DEL:esv4019342,IINS:nsv835171,DEL:esv4012499</t>
+  </si>
+  <si>
+    <t>DEL:esv4015056,INV:esv3896856,DEL:esv4014184,INV:esv3896874,INV:esv3896916,DEL:esv4015629,INV:esv3896785,INV:esv3896783</t>
+  </si>
+  <si>
+    <t>DEL:esv4012224,DEL:esv4016814,INV:esv3898433</t>
+  </si>
+  <si>
+    <t>DEL:nsv2728340,DEL:nsv2728353</t>
+  </si>
+  <si>
+    <t>Believed causal deletion of one bp. The deletion causes a premature terminaton which shortens the protein by 401 aa</t>
+  </si>
+  <si>
+    <t>Chondrodysplasia, recessive (Bulldog)</t>
+  </si>
+  <si>
+    <t>Chondrodysplasia</t>
+  </si>
+  <si>
+    <t>EVC2</t>
+  </si>
+  <si>
+    <t>Tyrolean Grey</t>
+  </si>
+  <si>
+    <t>c.2993_2994delAC</t>
+  </si>
+  <si>
+    <t>p.Asp998GlufsTer13</t>
+  </si>
+  <si>
+    <t>OMIA 000187-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000004277</t>
+  </si>
+  <si>
+    <t>Large SV. Comes from study on dairy cattle</t>
+  </si>
+  <si>
+    <t>Casual variant. a 2 bp deletion located in exon 19 of the bovine EVC2 gene causes a frame shift and thereby premature stop codon</t>
+  </si>
+  <si>
+    <t>DEL:esv4018357,DEL:4012036,DEL:esv4013733</t>
+  </si>
+  <si>
+    <t>Relativly small SVs (6-445 bp). Comes from study on dairy cattle</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>No but there are some IMPRECISE variants for BTA125,126, 127 and 130</t>
+  </si>
+  <si>
+    <t>No but there are some lowQual and IMPRECISE for BTA125,128, 127 and 130</t>
+  </si>
+  <si>
+    <t>No but there are some lowQual for BTA125,126, 128, 127 and 130</t>
+  </si>
+  <si>
+    <t>No, but there are LowQual for BTA128 and 131</t>
+  </si>
+  <si>
+    <t>Yes, BTA127(combined):INV00000602. There are other IMPRECISE and LowQual</t>
+  </si>
+  <si>
+    <t>BTA125(combined):DUP00002013. There are other IMPRECISE and LowQual</t>
+  </si>
+  <si>
+    <t>No but there are some IMPRECISE variants for BTA126, 127,128 and 129</t>
+  </si>
+  <si>
+    <t>No but there are some IMPRECISE variants for BTA126, 127,128 129 and 130</t>
+  </si>
+  <si>
+    <t>No but there are some LowQual</t>
+  </si>
+  <si>
+    <t>RDCSWEM000000085409:DEL00000236, RDCSWEM000000091804:DEL00000241, RDCSWEM000000093082:DEL00000266,BTA126(combined):DEL00002013,BTA128(combined):DEL00001972,BTA129(combined):DEL00001508</t>
   </si>
 </sst>
 </file>
@@ -3152,12 +3306,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Courier"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3170,10 +3318,15 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val=".Apple Symbols Fallback"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3255,7 +3408,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3279,15 +3432,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3317,9 +3468,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3891,12 +4039,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53E3D7F1-38C9-AB46-99BA-209E7F03E84D}" name="Tabell1" displayName="Tabell1" ref="A1:AD15" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A1:AD15" xr:uid="{0AA2673E-FE49-C747-96B4-3C5666F9D2F9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53E3D7F1-38C9-AB46-99BA-209E7F03E84D}" name="Tabell1" displayName="Tabell1" ref="A1:AD16" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A1:AD16" xr:uid="{0AA2673E-FE49-C747-96B4-3C5666F9D2F9}"/>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{ACE7D78E-E96B-1F4D-8067-F66CD3F7FD27}" name="BREED-VEXA" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{085AC52D-1D2E-754A-A01E-C239BDEE8C5D}" name="Chr" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{57DD89D0-BA8A-EC41-B6BE-5282B760D848}" name="SNP POS" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{57DD89D0-BA8A-EC41-B6BE-5282B760D848}" name="SNP/SV POS" dataDxfId="26"/>
     <tableColumn id="4" xr3:uid="{77F86C3C-CF5A-D34D-8A31-6F5D47D6EFA0}" name="GENE START" dataDxfId="25"/>
     <tableColumn id="28" xr3:uid="{4DA20CC4-1E0E-BB48-932D-5A43187A53BE}" name="GENE END" dataDxfId="24"/>
     <tableColumn id="5" xr3:uid="{9412F10F-D21D-B546-B7E1-92F91D306254}" name="OMIA" dataDxfId="23"/>
@@ -4226,75 +4374,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5724AFB8-EF24-374C-BA51-A6E5C12EB880}">
-  <dimension ref="A1:AD15"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="J9" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="62" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="71.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="90.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="62" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="64.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="72.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="77.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="33" customHeight="1">
+    <row r="1" spans="1:30" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>246</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>375</v>
+        <v>406</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>236</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="J1" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>370</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>376</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>247</v>
@@ -4303,88 +4455,90 @@
         <v>248</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="AD1" s="7" t="s">
-        <v>291</v>
-      </c>
     </row>
-    <row r="2" spans="1:30" s="13" customFormat="1" ht="51">
+    <row r="2" spans="1:30" s="6" customFormat="1" ht="51">
       <c r="A2" s="6" t="s">
         <v>239</v>
       </c>
       <c r="B2" s="6">
         <v>11</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>14742184</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>374</v>
+      <c r="D2" s="6">
+        <v>14696392</v>
+      </c>
+      <c r="E2" s="6">
+        <v>14751826</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>392</v>
-      </c>
       <c r="I2" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="J2" s="9"/>
+        <v>366</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>441</v>
+      </c>
       <c r="K2" s="6" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>237</v>
@@ -4393,42 +4547,40 @@
         <v>249</v>
       </c>
       <c r="N2" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>269</v>
       </c>
       <c r="V2" s="6">
         <v>11</v>
       </c>
       <c r="W2" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="X2" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="AB2" s="6">
         <v>2010</v>
@@ -4437,10 +4589,10 @@
         <v>19714378</v>
       </c>
       <c r="AD2" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="13" customFormat="1" ht="17">
+    <row r="3" spans="1:30" s="6" customFormat="1" ht="17">
       <c r="A3" s="6" t="s">
         <v>239</v>
       </c>
@@ -4457,20 +4609,22 @@
         <v>38676494</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>393</v>
+        <v>426</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="J3" s="6"/>
+        <v>373</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>442</v>
+      </c>
       <c r="K3" s="9" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>240</v>
@@ -4478,55 +4632,53 @@
       <c r="M3" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="N3" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="O3" s="15" t="s">
+      <c r="N3" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="Q3" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="S3" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="R3" s="6"/>
-      <c r="S3" s="15" t="s">
+      <c r="T3" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="V3" s="12">
+        <v>16</v>
+      </c>
+      <c r="W3" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="T3" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="U3" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="V3" s="15">
-        <v>16</v>
-      </c>
-      <c r="W3" s="15" t="s">
+      <c r="X3" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="Y3" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="AA3" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="15" t="s">
+      <c r="AB3" s="12">
+        <v>2002</v>
+      </c>
+      <c r="AC3" s="12">
+        <v>12466292</v>
+      </c>
+      <c r="AD3" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="AB3" s="15">
-        <v>2002</v>
-      </c>
-      <c r="AC3" s="15">
-        <v>12466292</v>
-      </c>
-      <c r="AD3" s="15" t="s">
-        <v>300</v>
-      </c>
     </row>
-    <row r="4" spans="1:30" s="13" customFormat="1">
+    <row r="4" spans="1:30" s="6" customFormat="1">
       <c r="A4" s="6" t="s">
         <v>239</v>
       </c>
@@ -4542,21 +4694,23 @@
       <c r="E4" s="6">
         <v>49629500</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>385</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>394</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15" t="s">
-        <v>380</v>
+      <c r="F4" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>374</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>237</v>
@@ -4564,55 +4718,53 @@
       <c r="M4" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="N4" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="O4" s="15" t="s">
+      <c r="N4" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="Q4" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="S4" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="V4" s="12">
+        <v>4</v>
+      </c>
+      <c r="W4" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="R4" s="6"/>
-      <c r="S4" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="T4" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="U4" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="V4" s="15">
-        <v>4</v>
-      </c>
-      <c r="W4" s="15" t="s">
+      <c r="X4" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="X4" s="15" t="s">
+      <c r="Y4" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="Y4" s="15" t="s">
+      <c r="AA4" s="12" t="s">
         <v>307</v>
       </c>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="15" t="s">
+      <c r="AB4" s="12">
+        <v>2016</v>
+      </c>
+      <c r="AC4" s="12">
+        <v>26992691</v>
+      </c>
+      <c r="AD4" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="AB4" s="15">
-        <v>2016</v>
-      </c>
-      <c r="AC4" s="15">
-        <v>26992691</v>
-      </c>
-      <c r="AD4" s="10" t="s">
-        <v>309</v>
-      </c>
     </row>
-    <row r="5" spans="1:30" s="13" customFormat="1">
+    <row r="5" spans="1:30" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
         <v>239</v>
       </c>
@@ -4620,7 +4772,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D5" s="6">
         <v>61599658</v>
@@ -4629,20 +4781,22 @@
         <v>61638727</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>391</v>
-      </c>
-      <c r="J5" s="6"/>
+        <v>385</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>440</v>
+      </c>
       <c r="K5" s="6" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>237</v>
@@ -4650,53 +4804,50 @@
       <c r="M5" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="N5" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="O5" s="15" t="s">
+      <c r="N5" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="P5" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="Q5" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="S5" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="V5" s="12">
+        <v>24</v>
+      </c>
+      <c r="W5" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="R5" s="6"/>
-      <c r="S5" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="T5" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="U5" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="V5" s="15">
-        <v>24</v>
-      </c>
-      <c r="W5" s="15" t="s">
+      <c r="X5" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="X5" s="15" t="s">
+      <c r="Y5" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="Y5" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="15">
+      <c r="AB5" s="12">
         <v>2007</v>
       </c>
-      <c r="AC5" s="15">
+      <c r="AC5" s="12">
         <v>17420465</v>
       </c>
-      <c r="AD5" s="15" t="s">
-        <v>274</v>
+      <c r="AD5" s="12" t="s">
+        <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="13" customFormat="1">
+    <row r="6" spans="1:30" s="6" customFormat="1">
       <c r="A6" s="6" t="s">
         <v>239</v>
       </c>
@@ -4704,7 +4855,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D6" s="6">
         <v>27116487</v>
@@ -4712,21 +4863,23 @@
       <c r="E6" s="6">
         <v>27131137</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>396</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>397</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>398</v>
-      </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15" t="s">
-        <v>399</v>
+      <c r="F6" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>391</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>241</v>
@@ -4734,45 +4887,38 @@
       <c r="M6" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="N6" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="O6" s="15" t="s">
+      <c r="N6" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="P6" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="Q6" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="S6" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="15" t="s">
+      <c r="T6" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="X6" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="T6" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="15" t="s">
+      <c r="Y6" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="Y6" s="15" t="s">
-        <v>325</v>
-      </c>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="15">
+      <c r="AB6" s="12">
         <v>2016</v>
       </c>
-      <c r="AC6" s="15">
+      <c r="AC6" s="12">
         <v>27364156</v>
       </c>
-      <c r="AD6" s="6"/>
     </row>
-    <row r="7" spans="1:30" s="13" customFormat="1">
+    <row r="7" spans="1:30" s="6" customFormat="1" ht="34">
       <c r="A7" s="6" t="s">
         <v>239</v>
       </c>
@@ -4782,16 +4928,29 @@
       <c r="C7" s="6">
         <v>63668380</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15" t="s">
+      <c r="D7" s="6">
+        <v>63650234</v>
+      </c>
+      <c r="E7" s="6">
+        <v>63696918</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>400</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>392</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>238</v>
@@ -4799,53 +4958,50 @@
       <c r="M7" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="N7" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="O7" s="15" t="s">
+      <c r="N7" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="Q7" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="S7" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="R7" s="6"/>
-      <c r="S7" s="15" t="s">
+      <c r="T7" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="V7" s="12">
+        <v>17</v>
+      </c>
+      <c r="W7" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="T7" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="U7" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="V7" s="15">
-        <v>17</v>
-      </c>
-      <c r="W7" s="15" t="s">
+      <c r="Y7" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="15" t="s">
+      <c r="AA7" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="15" t="s">
+      <c r="AB7" s="12">
+        <v>2014</v>
+      </c>
+      <c r="AC7" s="12">
+        <v>25306138</v>
+      </c>
+      <c r="AD7" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="AB7" s="15">
-        <v>2014</v>
-      </c>
-      <c r="AC7" s="15">
-        <v>25306138</v>
-      </c>
-      <c r="AD7" s="10" t="s">
-        <v>334</v>
-      </c>
     </row>
-    <row r="8" spans="1:30" s="13" customFormat="1" ht="34">
+    <row r="8" spans="1:30" s="6" customFormat="1" ht="34">
       <c r="A8" s="6" t="s">
         <v>239</v>
       </c>
@@ -4853,7 +5009,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D8" s="6">
         <v>50994444</v>
@@ -4861,21 +5017,23 @@
       <c r="E8" s="6">
         <v>51122558</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>401</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>403</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>404</v>
-      </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15" t="s">
-        <v>402</v>
+      <c r="F8" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>394</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>238</v>
@@ -4883,45 +5041,38 @@
       <c r="M8" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="N8" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="O8" s="15" t="s">
+      <c r="N8" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="Q8" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="Q8" s="15" t="s">
+      <c r="S8" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="V8" s="12">
+        <v>3</v>
+      </c>
+      <c r="Z8" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="R8" s="6"/>
-      <c r="S8" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="T8" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="U8" s="6"/>
-      <c r="V8" s="15">
-        <v>3</v>
-      </c>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="15" t="s">
+      <c r="AB8" s="12">
+        <v>2017</v>
+      </c>
+      <c r="AC8" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="15">
-        <v>2017</v>
-      </c>
-      <c r="AC8" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="AD8" s="6"/>
     </row>
-    <row r="9" spans="1:30" s="13" customFormat="1" ht="34">
+    <row r="9" spans="1:30" s="6" customFormat="1" ht="17">
       <c r="A9" s="6" t="s">
         <v>239</v>
       </c>
@@ -4929,29 +5080,31 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
+      </c>
+      <c r="D9" s="6">
+        <v>42811272</v>
+      </c>
+      <c r="E9" s="6">
+        <v>47002161</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="J9" s="9"/>
+        <v>310</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>446</v>
+      </c>
       <c r="K9" s="9" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>238</v>
@@ -4960,46 +5113,46 @@
         <v>256</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O9" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="P9" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="P9" s="15" t="s">
-        <v>343</v>
-      </c>
       <c r="Q9" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="V9" s="6">
         <v>7</v>
       </c>
       <c r="W9" s="6" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Y9" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Z9" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AA9" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AB9" s="6">
         <v>2011</v>
@@ -5008,294 +5161,399 @@
         <v>22118103</v>
       </c>
       <c r="AD9" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="13" customFormat="1">
+    <row r="10" spans="1:30" s="6" customFormat="1" ht="34">
       <c r="A10" s="6" t="s">
         <v>239</v>
       </c>
       <c r="B10" s="6">
         <v>19</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="6">
         <v>10833921</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="16" t="s">
-        <v>352</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="D10" s="6">
+        <v>10816976</v>
+      </c>
+      <c r="E10" s="6">
+        <v>10840892</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>405</v>
+      </c>
       <c r="L10" s="6" t="s">
         <v>242</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="N10" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>342</v>
-      </c>
-      <c r="P10" s="16" t="s">
+      <c r="N10" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q10" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="Q10" s="16" t="s">
+      <c r="S10" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="T10" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="U10" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="V10" s="12">
+        <v>19</v>
+      </c>
+      <c r="W10" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="R10" s="8"/>
-      <c r="S10" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="T10" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="U10" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="V10" s="16">
-        <v>19</v>
-      </c>
-      <c r="W10" s="16" t="s">
+      <c r="X10" s="12" t="s">
         <v>347</v>
       </c>
-      <c r="X10" s="16" t="s">
+      <c r="Y10" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="Y10" s="16" t="s">
+      <c r="AA10" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="16" t="s">
+      <c r="AB10" s="12">
+        <v>2016</v>
+      </c>
+      <c r="AC10" s="12">
+        <v>27225349</v>
+      </c>
+      <c r="AD10" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="AB10" s="16">
-        <v>2016</v>
-      </c>
-      <c r="AC10" s="16">
-        <v>27225349</v>
-      </c>
-      <c r="AD10" s="17" t="s">
-        <v>351</v>
-      </c>
     </row>
-    <row r="11" spans="1:30" s="13" customFormat="1">
+    <row r="11" spans="1:30" s="6" customFormat="1" ht="51">
       <c r="A11" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="B11" s="6">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D11" s="6">
+        <v>20346401</v>
+      </c>
+      <c r="E11" s="6">
+        <v>20423092</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>410</v>
+      </c>
       <c r="L11" s="6" t="s">
         <v>238</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="N11" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="O11" s="16" t="s">
+      <c r="N11" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="P11" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="P11" s="16" t="s">
+      <c r="Q11" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="Q11" s="16" t="s">
+      <c r="S11" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="R11" s="8"/>
-      <c r="S11" s="16" t="s">
+      <c r="T11" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z11" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="T11" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="16" t="s">
-        <v>357</v>
-      </c>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="16">
+      <c r="AB11" s="12">
         <v>2014</v>
       </c>
-      <c r="AC11" s="16">
+      <c r="AC11" s="12">
         <v>24391517</v>
       </c>
-      <c r="AD11" s="8"/>
     </row>
-    <row r="12" spans="1:30" s="13" customFormat="1" ht="51">
+    <row r="12" spans="1:30" s="6" customFormat="1" ht="187">
       <c r="A12" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="9" t="s">
-        <v>368</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="B12" s="6">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F12" t="s">
+        <v>413</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>419</v>
+      </c>
       <c r="L12" s="6" t="s">
         <v>243</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
+      <c r="N12" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q12" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="R12" s="8"/>
+      <c r="S12" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="T12" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="U12" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="V12" s="14">
+        <v>23</v>
+      </c>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="14">
+        <v>2016</v>
+      </c>
+      <c r="AC12" s="14">
+        <v>27091210</v>
+      </c>
+      <c r="AD12" s="8"/>
     </row>
-    <row r="13" spans="1:30" s="13" customFormat="1">
+    <row r="13" spans="1:30" s="6" customFormat="1" ht="34">
       <c r="A13" s="6" t="s">
         <v>239</v>
       </c>
       <c r="B13" s="6">
         <v>13</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="6">
         <v>24024659</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="D13" s="6">
+        <v>23964738</v>
+      </c>
+      <c r="E13" s="6">
+        <v>24056173</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>427</v>
+      </c>
       <c r="L13" s="6" t="s">
         <v>244</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="N13" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="O13" s="16" t="s">
+      <c r="N13" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="P13" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="P13" s="16" t="s">
+      <c r="Q13" s="12" t="s">
         <v>360</v>
       </c>
-      <c r="Q13" s="16" t="s">
+      <c r="S13" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="T13" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="U13" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="V13" s="12">
+        <v>13</v>
+      </c>
+      <c r="W13" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="R13" s="8"/>
-      <c r="S13" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="T13" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="U13" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="V13" s="16">
-        <v>13</v>
-      </c>
-      <c r="W13" s="16" t="s">
+      <c r="X13" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="X13" s="16" t="s">
+      <c r="Y13" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="Y13" s="16" t="s">
+      <c r="AA13" s="12" t="s">
         <v>364</v>
       </c>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="AB13" s="16">
+      <c r="AB13" s="12">
         <v>2016</v>
       </c>
-      <c r="AC13" s="16">
+      <c r="AC13" s="12">
         <v>26923438</v>
       </c>
-      <c r="AD13" s="17" t="s">
-        <v>351</v>
+      <c r="AD13" s="10" t="s">
+        <v>350</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="13" customFormat="1">
+    <row r="14" spans="1:30" s="6" customFormat="1" ht="34">
       <c r="A14" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="B14" s="6">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14" s="6">
+        <v>103500611</v>
+      </c>
+      <c r="E14" s="6">
+        <v>103662790</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>437</v>
+      </c>
       <c r="L14" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="M14" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
+      <c r="M14" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="AB14" s="6">
+        <v>2014</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>24733244</v>
+      </c>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="6"/>
@@ -5311,26 +5569,64 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
-      <c r="AA15" s="6"/>
-      <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="6"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="8"/>
+    </row>
+    <row r="16" spans="1:30">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="I26" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="AD4" r:id="rId1" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{6FB82143-03EF-B943-B3B6-9B4DAEF5B546}"/>
     <hyperlink ref="AD7" r:id="rId2" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{B60A99FD-0C8B-EC4B-A9FA-00FD4C228C68}"/>
@@ -5338,6 +5634,7 @@
     <hyperlink ref="AD13" r:id="rId4" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{10561EFE-5896-9F41-A883-2CDD80893631}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
   </tableParts>
@@ -5348,7 +5645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B96105-ED37-6A48-B14A-8CDBB38B2477}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
@@ -5358,10 +5655,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5378,24 +5675,24 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="25" t="s">
+      <c r="J2" s="24"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="27"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:13" ht="34">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
Continuing looking at Holstein traits
</commit_message>
<xml_diff>
--- a/SVs_identification/results/Summary of monogenous traits.xlsx
+++ b/SVs_identification/results/Summary of monogenous traits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/breedmaps/SVs_identification/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A54BBD-5BA4-B947-B6E2-6D68B2B0BAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14D2EAB-7830-474E-BF0F-8F0D696195AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{000CD8DE-5782-4E40-B73D-11CA3F163355}"/>
+    <workbookView xWindow="12220" yWindow="500" windowWidth="16580" windowHeight="16380" xr2:uid="{000CD8DE-5782-4E40-B73D-11CA3F163355}"/>
   </bookViews>
   <sheets>
     <sheet name="All info" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="672">
   <si>
     <r>
       <rPr>
@@ -2497,9 +2497,6 @@
   </si>
   <si>
     <t>Chr</t>
-  </si>
-  <si>
-    <t>Phenotype</t>
   </si>
   <si>
     <t>Disease</t>
@@ -3226,6 +3223,746 @@
   </si>
   <si>
     <t>RDCSWEM000000085409:DEL00000236, RDCSWEM000000091804:DEL00000241, RDCSWEM000000093082:DEL00000266,BTA126(combined):DEL00002013,BTA128(combined):DEL00001972,BTA129(combined):DEL00001508</t>
+  </si>
+  <si>
+    <t>Phenotype when homozygot</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Carlito"/>
+        <family val="2"/>
+      </rPr>
+      <t>Factor XI deficiency (blood clotting disorder)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (also when homozygot)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Carlito"/>
+        <family val="2"/>
+      </rPr>
+      <t>Red factor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Svart/vit pälsfärg when heterozygot)</t>
+    </r>
+  </si>
+  <si>
+    <t>Fleckvieh, Holstein-Friesian, Jersey</t>
+  </si>
+  <si>
+    <t>Leukocyte adhesion deficiency, type I</t>
+  </si>
+  <si>
+    <t>ITGB2</t>
+  </si>
+  <si>
+    <t>g.145114963A&gt;G</t>
+  </si>
+  <si>
+    <t>c.383A&gt;G</t>
+  </si>
+  <si>
+    <t>p.D128G</t>
+  </si>
+  <si>
+    <t>rs445709131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+OMIA 000595-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000017060</t>
+  </si>
+  <si>
+    <t>DEL:esv4015512,DEL:esv4013947,DEL:esv4017519,DEL:esv4017704,INS:nsv810758</t>
+  </si>
+  <si>
+    <t>Big SVs (~100 000-150 000 000). Comes from studies on dairy cattle</t>
+  </si>
+  <si>
+    <t>Probable causal SNP. Found in only 4 Holstein</t>
+  </si>
+  <si>
+    <t>Friesian, Holstein</t>
+  </si>
+  <si>
+    <t>Complex vertebral malformation</t>
+  </si>
+  <si>
+    <t>SLC35A3</t>
+  </si>
+  <si>
+    <t>g.43412427G&gt;T</t>
+  </si>
+  <si>
+    <t>c.538G&gt;T</t>
+  </si>
+  <si>
+    <t>p.V180F</t>
+  </si>
+  <si>
+    <t>rs438228855</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000012454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+OMIA 001340-9913</t>
+  </si>
+  <si>
+    <t>DEL:esv4015120</t>
+  </si>
+  <si>
+    <t>A big SV ~80 000 000 bp. Comes from study on dairy cattle</t>
+  </si>
+  <si>
+    <t>Causal SNP. Nonsense mutation in SLC35A3 gene</t>
+  </si>
+  <si>
+    <t>OMIA 001935-9913</t>
+  </si>
+  <si>
+    <t>Fleckvieh</t>
+  </si>
+  <si>
+    <t>Zinc deficiency-like syndrome</t>
+  </si>
+  <si>
+    <t>PLD4</t>
+  </si>
+  <si>
+    <t>g.71001232G&gt;A</t>
+  </si>
+  <si>
+    <t>c.702G&gt;A</t>
+  </si>
+  <si>
+    <t>p.W234*</t>
+  </si>
+  <si>
+    <t>rs378824791</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000015160</t>
+  </si>
+  <si>
+    <t>Causal SNP. Stop gain  in PLD4 gene</t>
+  </si>
+  <si>
+    <t>Syndactylism (Mulefoot)</t>
+  </si>
+  <si>
+    <t>Holstein</t>
+  </si>
+  <si>
+    <t>Syndactyly (mule foot)</t>
+  </si>
+  <si>
+    <t>LRP4</t>
+  </si>
+  <si>
+    <t>delins, small (&lt;=20)</t>
+  </si>
+  <si>
+    <t>ARS-UCD1.2</t>
+  </si>
+  <si>
+    <t>g.76800972_76800973delCGinsAT</t>
+  </si>
+  <si>
+    <t>c.4863_4864delCGinsAT</t>
+  </si>
+  <si>
+    <t>p.(Asn1621_Gly1622delinsLysCys</t>
+  </si>
+  <si>
+    <t>Variant information updated to ARS-UCD1.2 and variant effect predicted using Ensembl Variant Effect Predictor (VEP) based on transcript ENSBTAT00000043997.4</t>
+  </si>
+  <si>
+    <t>OMIA 000963-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000008429</t>
+  </si>
+  <si>
+    <t>CNV:nsv2728302,INS:nsv810217,DEL:esv4013079,DEL:esv4015521</t>
+  </si>
+  <si>
+    <t>Big CNVs. Comes from studies on beef, dairy or mixed cattle</t>
+  </si>
+  <si>
+    <t>Probable causal SNP. Missense mutation in LRP4 gene</t>
+  </si>
+  <si>
+    <t>Brachyspina</t>
+  </si>
+  <si>
+    <t>FANCI</t>
+  </si>
+  <si>
+    <t>g.21184870_21188198del</t>
+  </si>
+  <si>
+    <t>c.526-64495_526-67824del</t>
+  </si>
+  <si>
+    <t>p.V877Lfs27X</t>
+  </si>
+  <si>
+    <t>Breed and variant information kindly provided or confirmed by Matt McClure and Jennifer McClure from "Understanding Genetics and Complete Genetic Disease and Trait Definition (Expanded 2016 Edition)" (https://www.icbf.com/wp/?page_id=2170)</t>
+  </si>
+  <si>
+    <t>OMIA 000151-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000009097</t>
+  </si>
+  <si>
+    <t>INV:esv3897707,DEL:esv4013971</t>
+  </si>
+  <si>
+    <t>Large INV(31 mil bp) and relatively big del(~3000bp). Comes from studies on dairy cattle</t>
+  </si>
+  <si>
+    <t>Cluster of possible causal regions. Later found causal deletion ~330 kb</t>
+  </si>
+  <si>
+    <t>Friesian, Holstein, Holstein-Friesian, Red Holstein, Wagyu</t>
+  </si>
+  <si>
+    <t>Deficiency of uridine monophosphate synthase</t>
+  </si>
+  <si>
+    <t>UMPS</t>
+  </si>
+  <si>
+    <t>g.69756880C&gt;T</t>
+  </si>
+  <si>
+    <t>c.1213C&gt;T</t>
+  </si>
+  <si>
+    <t>p.R405*</t>
+  </si>
+  <si>
+    <t>OMIA 000262-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000013727</t>
+  </si>
+  <si>
+    <t>DEL:esv4015512, DEL:esv4013408, DEL:esv4013947, DEL:esv4011790, DEL:esv4012073, DEL:esv4017070,INV:esv3897631, DEL:esv4015386,DEL:esv4017519,DEL:nsv2727911,CNV:nsv2728100,DEL:esv4017704,INV:esv3897556,DEL:nsv2727644</t>
+  </si>
+  <si>
+    <t>Big and small CNVs and INV. Comes from studies on dairy cattle expect on done on beef cattle</t>
+  </si>
+  <si>
+    <t>The only known casual mutation is a missense mutation in UMPS gene</t>
+  </si>
+  <si>
+    <t>Holstein-Friesian</t>
+  </si>
+  <si>
+    <t>Citrullinaemia</t>
+  </si>
+  <si>
+    <t>ASS1</t>
+  </si>
+  <si>
+    <t>g.100802781C&gt;T</t>
+  </si>
+  <si>
+    <t>c.256C&gt;T</t>
+  </si>
+  <si>
+    <t>p.R86*</t>
+  </si>
+  <si>
+    <t>OMIA 000194-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000020747</t>
+  </si>
+  <si>
+    <t>Probably because of a nonsense mutation in the 5th of 9 exons of the ASS gene.</t>
+  </si>
+  <si>
+    <t>Holstein, Sahiwal</t>
+  </si>
+  <si>
+    <t>Factor XI deficiency</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>insertion, gross (&gt;20)</t>
+  </si>
+  <si>
+    <t>Variant information kindly provided or confirmed by Hubert Pausch, including information from Additional Table 6 of Jansen et al. (2013) BMC Genomics201314:446 https://doi.org/10.1186/1471-2164-14-446</t>
+  </si>
+  <si>
+    <t>insertion, gross(&lt;20)</t>
+  </si>
+  <si>
+    <t>a 76-bp insertion in exon 12 of the Factor XI gene,
+200922: g. and c. info moved here (g.15367048; c.1406ins76) until can be standardised</t>
+  </si>
+  <si>
+    <t>76 bp insertion. Unclear location since it was identified in previous reference genomes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+OMIA 000363-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000003572</t>
+  </si>
+  <si>
+    <t>Holstein cholesterol deficiency</t>
+  </si>
+  <si>
+    <t>APOB</t>
+  </si>
+  <si>
+    <t>"1.3kb insertion of a transposable LTR element (ERV2-1) in the coding sequence of the APOB gene, which leads to truncated transcripts and aberrant splicing [p.Gly135ValfsX10)]"</t>
+  </si>
+  <si>
+    <t>OMIA 001965-9913</t>
+  </si>
+  <si>
+    <t>INS:nsv1302963</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000008505</t>
+  </si>
+  <si>
+    <t>"A transposable element (LTR) insertion(ERV2-1) in APOB causes cholesterol deficiency (CD) in Holstein cattle."</t>
+  </si>
+  <si>
+    <t>77891733-77891734</t>
+  </si>
+  <si>
+    <t>OMIA 000515-9913</t>
+  </si>
+  <si>
+    <t>Abortion due to a nonsense mutation in APAF1 on haplotype HH1</t>
+  </si>
+  <si>
+    <t>APAF1</t>
+  </si>
+  <si>
+    <t>g.63150400C&gt;T</t>
+  </si>
+  <si>
+    <t>c.1741C&gt;T</t>
+  </si>
+  <si>
+    <t>p.Q581*</t>
+  </si>
+  <si>
+    <t>rs448942533</t>
+  </si>
+  <si>
+    <t>OMIA 000001-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000021661</t>
+  </si>
+  <si>
+    <t>DEL:nsv2727702,DEL:esv4016199,DEL:esv4017675</t>
+  </si>
+  <si>
+    <t>Large DEL(33, 33 and 90 mil bp). Comes from beef and dairy studies</t>
+  </si>
+  <si>
+    <t>A nonsense mutation in APAF1 which truncates the protein</t>
+  </si>
+  <si>
+    <t>94,860,836 to 96,553,339 (UMD3.1)</t>
+  </si>
+  <si>
+    <t>No casual variant has been identified after an extensive study</t>
+  </si>
+  <si>
+    <t>OMIA 001823-9913</t>
+  </si>
+  <si>
+    <t>Abortion due to haplotype HH3</t>
+  </si>
+  <si>
+    <t>SMC2</t>
+  </si>
+  <si>
+    <t>g.95410507T&gt;C</t>
+  </si>
+  <si>
+    <t>c.3404T&gt;C</t>
+  </si>
+  <si>
+    <t>p.F1135S</t>
+  </si>
+  <si>
+    <t>rs456206907</t>
+  </si>
+  <si>
+    <t>OMIA 001824-9913</t>
+  </si>
+  <si>
+    <t>Causal SNP. Lethal mutation in SMC2 gene</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000008772</t>
+  </si>
+  <si>
+    <t>DEL:esv4016142</t>
+  </si>
+  <si>
+    <t>Large deletion. Comes from study on dairy cattle</t>
+  </si>
+  <si>
+    <t>Abortion due to haplotype HH4</t>
+  </si>
+  <si>
+    <t>GART</t>
+  </si>
+  <si>
+    <t>g.1277227A&gt;C</t>
+  </si>
+  <si>
+    <t>c.869A&gt;C</t>
+  </si>
+  <si>
+    <t>p.N290T</t>
+  </si>
+  <si>
+    <t>rs465495560</t>
+  </si>
+  <si>
+    <t>OMIA 001826-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000009188</t>
+  </si>
+  <si>
+    <t>Probable causal SNP. Effects fertility</t>
+  </si>
+  <si>
+    <t>Abortion due to haplotype HH5</t>
+  </si>
+  <si>
+    <t>TFB1M</t>
+  </si>
+  <si>
+    <t>complex rearrangement</t>
+  </si>
+  <si>
+    <t>"a deletion of 138kbp, spanning position 93,233kb to 93,371kb on chromosome 9 (BTA9), harboring only dimethyl-adenosine transferase 1 (TFB1M). The deletion breakpoints are flanked by bovine long interspersed nuclear elements Bov-B (upstream) and L1ME3 (downstream), suggesting a homologous recombination/deletion event."</t>
+  </si>
+  <si>
+    <t>OMIA 001941-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000031895</t>
+  </si>
+  <si>
+    <t>DEL:esv4012526</t>
+  </si>
+  <si>
+    <t>Abortion due to haplotype HH6</t>
+  </si>
+  <si>
+    <t>SDE2</t>
+  </si>
+  <si>
+    <t>start-lost</t>
+  </si>
+  <si>
+    <t>g.29773628A&gt;G</t>
+  </si>
+  <si>
+    <t>"This A-to-G transition changes the initiator ATG (methionine) codon to ACG because the gene is transcribed on the reverse strand. . . . Initiation of translation at the closest in-frame Met codon would truncate SDE2 by 83 amino acids, including an 8-amino acid motif conserved among eukaryotes"</t>
+  </si>
+  <si>
+    <t>rs434666183</t>
+  </si>
+  <si>
+    <t>OMIA 002149-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000012787</t>
+  </si>
+  <si>
+    <t>Probable SNP which causes a start codon to form</t>
+  </si>
+  <si>
+    <t>Causal deletion verified by knock out mice on TFB1M</t>
+  </si>
+  <si>
+    <t>Large deletions. Comes from studies on beef cattle</t>
+  </si>
+  <si>
+    <t>Abortion due to haplotype HH7</t>
+  </si>
+  <si>
+    <t>CENPU</t>
+  </si>
+  <si>
+    <t>g.14168130_14168133delTACT</t>
+  </si>
+  <si>
+    <t>Hozé et al. (2019): "Considering that CENPU is transcribed in the antisense orientation, this mutation is predicted to result in deletion of the nucleotides located at position +3 to + 6 bp after the splicing donor site of exon 11. Using cross-species nucleotide alignment, we observed that the nucleotide at position +3 is entirely conserved among vertebrates . . . , which suggests that it plays an important role in regulation of CENPU splicing. If modified after exon 11, the abnormal splicing of CENPU could cause mRNA decay or the production of a protein modified after residue 319 out of 409 AA. Based on these factors, we assumed that mutation g.14168130_14168133delTACT on chromosome 27 alters the splicing of CENPU and is embryonic lethal."</t>
+  </si>
+  <si>
+    <t>OMIA 001830-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000018864</t>
+  </si>
+  <si>
+    <t>DEL:nsv2727371,CNV:nsv810717,CNV:nsv811031</t>
+  </si>
+  <si>
+    <t>Large CNVs. Del ~7000bp. Comes from beef cattle</t>
+  </si>
+  <si>
+    <t>Likely causal 4 bp deletion which is conserved in mammals. Check 19 breeds but only Holstein ahd the deletion</t>
+  </si>
+  <si>
+    <t>Bulldog calf</t>
+  </si>
+  <si>
+    <t>COL2A1</t>
+  </si>
+  <si>
+    <t>g.32301911_32308589del6679</t>
+  </si>
+  <si>
+    <t>"Sanger sequencing revealed the precise breakpoints of the heterozygous deletion from position 32 301 911 located in intron 25 to 32 308 589 located within exon 45. The 6679 bp deletion includes the entire sequence of 18 exons (26–44) plus the first 36 nucleotides of exon 45" (Jacinto et al., 2020)</t>
+  </si>
+  <si>
+    <t>delins, gross (&gt;20)</t>
+  </si>
+  <si>
+    <t>g.32303127_32306640delinsTCTGGGGAGC</t>
+  </si>
+  <si>
+    <t>Charolais, Salers</t>
+  </si>
+  <si>
+    <t>g.32469820G&gt;A</t>
+  </si>
+  <si>
+    <t>c.1791G&gt;A</t>
+  </si>
+  <si>
+    <t>p.G600D</t>
+  </si>
+  <si>
+    <t>g.32471813G&gt;A</t>
+  </si>
+  <si>
+    <t>c.2158G&gt;A</t>
+  </si>
+  <si>
+    <t>p.G720S</t>
+  </si>
+  <si>
+    <t>Danish Holstein</t>
+  </si>
+  <si>
+    <t>bulldog calf</t>
+  </si>
+  <si>
+    <t>g.32473300G&gt;A</t>
+  </si>
+  <si>
+    <t>c.2463+1G&gt;A</t>
+  </si>
+  <si>
+    <t>g.32475732G&gt;A</t>
+  </si>
+  <si>
+    <t>p.G960R</t>
+  </si>
+  <si>
+    <t>g.32476082G&gt;A</t>
+  </si>
+  <si>
+    <t>c.2986G&gt;A</t>
+  </si>
+  <si>
+    <t>p.G996S</t>
+  </si>
+  <si>
+    <t>rs876243579</t>
+  </si>
+  <si>
+    <t>g.32476808G&gt;A</t>
+  </si>
+  <si>
+    <t>c.3166G&gt;A</t>
+  </si>
+  <si>
+    <t>p.Gly1056Ser</t>
+  </si>
+  <si>
+    <t>OMIA 001926-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000013155</t>
+  </si>
+  <si>
+    <t>DEL:nsv2727702,INV:esv3898479</t>
+  </si>
+  <si>
+    <t>Large CNVs. Comes from studies on beef respectively dairy cattle</t>
+  </si>
+  <si>
+    <t>32303127-32306640</t>
+  </si>
+  <si>
+    <t>32301911-32308589</t>
+  </si>
+  <si>
+    <t>HOL</t>
+  </si>
+  <si>
+    <t>Dominant red</t>
+  </si>
+  <si>
+    <t>COPA</t>
+  </si>
+  <si>
+    <t>DR^DR</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>g.9479761C&gt;T</t>
+  </si>
+  <si>
+    <t>c.478C&gt;T</t>
+  </si>
+  <si>
+    <t>p.R160C</t>
+  </si>
+  <si>
+    <t>OMIA 001529-9913</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recto-vaginal constriction (RVC)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jersey Haplotype 1 (JH1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jersey Haplotype 2 (JH2)</t>
+    </r>
+  </si>
+  <si>
+    <t>OMIA 000850-9913</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>Abortion due to haplotype JH1</t>
+  </si>
+  <si>
+    <t>CWC15</t>
+  </si>
+  <si>
+    <t>g.15707169C&gt;T</t>
+  </si>
+  <si>
+    <t>c.163C&gt;T</t>
+  </si>
+  <si>
+    <t>p.R55*</t>
+  </si>
+  <si>
+    <t>OMIA 001697-9913</t>
+  </si>
+  <si>
+    <t>ENSBTAG00000007913</t>
+  </si>
+  <si>
+    <t>CNV:nsv2728302,DEL:esv4015884,DEL:nsv2728275,DEL:esv4015196</t>
+  </si>
+  <si>
+    <t>Large CNVs. Comes from studies on dairy and beef cattle</t>
+  </si>
+  <si>
+    <t>Causal SNP. Stop gain  in CWC15 gene</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,812,759 – 9,414,082bp (Wrong reference?)</t>
+  </si>
+  <si>
+    <t>OMIA001942-9913</t>
   </si>
 </sst>
 </file>
@@ -3408,7 +4145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3439,6 +4176,11 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3469,6 +4211,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -4039,8 +4783,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53E3D7F1-38C9-AB46-99BA-209E7F03E84D}" name="Tabell1" displayName="Tabell1" ref="A1:AD16" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A1:AD16" xr:uid="{0AA2673E-FE49-C747-96B4-3C5666F9D2F9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53E3D7F1-38C9-AB46-99BA-209E7F03E84D}" name="Tabell1" displayName="Tabell1" ref="A1:AD45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A1:AD45" xr:uid="{0AA2673E-FE49-C747-96B4-3C5666F9D2F9}"/>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{ACE7D78E-E96B-1F4D-8067-F66CD3F7FD27}" name="BREED-VEXA" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{085AC52D-1D2E-754A-A01E-C239BDEE8C5D}" name="Chr" dataDxfId="27"/>
@@ -4053,7 +4797,7 @@
     <tableColumn id="8" xr3:uid="{4D5D90D2-809A-DD43-BA84-6410B63686C1}" name="ENSEMBL GENOMIC CONTEXT FOR GENE" dataDxfId="21"/>
     <tableColumn id="27" xr3:uid="{FD14AF90-18C2-BA4A-A141-A4352E62B16A}" name="VARIANTS FOUND IN DATA" dataDxfId="20"/>
     <tableColumn id="29" xr3:uid="{0B49611E-A656-1B47-897D-7A419E74B73E}" name="RELEVANCE" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{8DAC3CF8-AB71-414D-8C5D-72830C12654B}" name="Phenotype" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{8DAC3CF8-AB71-414D-8C5D-72830C12654B}" name="Phenotype when homozygot" dataDxfId="18"/>
     <tableColumn id="7" xr3:uid="{58DF4A99-1410-7942-99C6-51B763D195AF}" name="Disease" dataDxfId="17"/>
     <tableColumn id="9" xr3:uid="{3E2DA18C-B667-C24C-A598-7BD04D408FDE}" name="Species Name" dataDxfId="16"/>
     <tableColumn id="10" xr3:uid="{B3EE0EC0-4AD8-394E-A5FE-757BE0A69B6C}" name="Breed(s)" dataDxfId="15"/>
@@ -4374,10 +5118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5724AFB8-EF24-374C-BA51-A6E5C12EB880}">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J9" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4391,7 +5135,7 @@
     <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="60.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="71.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="199.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="90.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="62" bestFit="1" customWidth="1"/>
@@ -4416,94 +5160,94 @@
   <sheetData>
     <row r="1" spans="1:30" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>246</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>236</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L1" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>248</v>
-      </c>
       <c r="N1" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>289</v>
-      </c>
-      <c r="AD1" s="7" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="6" customFormat="1" ht="51">
@@ -4523,64 +5267,64 @@
         <v>14751826</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>237</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N2" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>267</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>268</v>
       </c>
       <c r="V2" s="6">
         <v>11</v>
       </c>
       <c r="W2" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="X2" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="AB2" s="6">
         <v>2010</v>
@@ -4589,7 +5333,7 @@
         <v>19714378</v>
       </c>
       <c r="AD2" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:30" s="6" customFormat="1" ht="17">
@@ -4609,64 +5353,64 @@
         <v>38676494</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>240</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O3" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="S3" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="S3" s="12" t="s">
-        <v>294</v>
-      </c>
       <c r="T3" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="U3" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="U3" s="12" t="s">
-        <v>268</v>
       </c>
       <c r="V3" s="12">
         <v>16</v>
       </c>
       <c r="W3" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="X3" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="Y3" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="AA3" s="12" t="s">
         <v>297</v>
-      </c>
-      <c r="AA3" s="12" t="s">
-        <v>298</v>
       </c>
       <c r="AB3" s="12">
         <v>2002</v>
@@ -4675,7 +5419,7 @@
         <v>12466292</v>
       </c>
       <c r="AD3" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="6" customFormat="1">
@@ -4695,64 +5439,64 @@
         <v>49629500</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>237</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O4" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="Q4" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="Q4" s="12" t="s">
-        <v>303</v>
-      </c>
       <c r="S4" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="T4" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="T4" s="12" t="s">
+      <c r="U4" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>268</v>
       </c>
       <c r="V4" s="12">
         <v>4</v>
       </c>
       <c r="W4" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="X4" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="X4" s="12" t="s">
+      <c r="Y4" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="Y4" s="12" t="s">
+      <c r="AA4" s="12" t="s">
         <v>306</v>
-      </c>
-      <c r="AA4" s="12" t="s">
-        <v>307</v>
       </c>
       <c r="AB4" s="12">
         <v>2016</v>
@@ -4761,7 +5505,7 @@
         <v>26992691</v>
       </c>
       <c r="AD4" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:30" s="6" customFormat="1">
@@ -4772,7 +5516,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D5" s="6">
         <v>61599658</v>
@@ -4781,61 +5525,61 @@
         <v>61638727</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>385</v>
-      </c>
       <c r="J5" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>237</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O5" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="P5" s="12" t="s">
         <v>312</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="Q5" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="Q5" s="12" t="s">
-        <v>314</v>
-      </c>
       <c r="S5" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="T5" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="U5" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="U5" s="12" t="s">
-        <v>268</v>
       </c>
       <c r="V5" s="12">
         <v>24</v>
       </c>
       <c r="W5" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="X5" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="Y5" s="12" t="s">
         <v>316</v>
-      </c>
-      <c r="Y5" s="12" t="s">
-        <v>317</v>
       </c>
       <c r="AB5" s="12">
         <v>2007</v>
@@ -4844,7 +5588,7 @@
         <v>17420465</v>
       </c>
       <c r="AD5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:30" s="6" customFormat="1">
@@ -4855,7 +5599,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D6" s="6">
         <v>27116487</v>
@@ -4864,52 +5608,52 @@
         <v>27131137</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G6" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="I6" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="J6" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>390</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>391</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>241</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O6" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="P6" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="Q6" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="S6" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="S6" s="12" t="s">
+      <c r="T6" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="X6" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="T6" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="X6" s="12" t="s">
+      <c r="Y6" s="12" t="s">
         <v>323</v>
-      </c>
-      <c r="Y6" s="12" t="s">
-        <v>324</v>
       </c>
       <c r="AB6" s="12">
         <v>2016</v>
@@ -4935,61 +5679,61 @@
         <v>63696918</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>401</v>
-      </c>
       <c r="J7" s="12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>238</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O7" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="S7" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="S7" s="12" t="s">
-        <v>329</v>
-      </c>
       <c r="T7" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="U7" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="U7" s="12" t="s">
-        <v>268</v>
       </c>
       <c r="V7" s="12">
         <v>17</v>
       </c>
       <c r="W7" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="Y7" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="Y7" s="12" t="s">
+      <c r="AA7" s="12" t="s">
         <v>331</v>
-      </c>
-      <c r="AA7" s="12" t="s">
-        <v>332</v>
       </c>
       <c r="AB7" s="12">
         <v>2014</v>
@@ -4998,7 +5742,7 @@
         <v>25306138</v>
       </c>
       <c r="AD7" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:30" s="6" customFormat="1" ht="34">
@@ -5009,7 +5753,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D8" s="6">
         <v>50994444</v>
@@ -5018,58 +5762,58 @@
         <v>51122558</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G8" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="K8" s="12" t="s">
         <v>393</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>394</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>238</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O8" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="Q8" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="Q8" s="12" t="s">
-        <v>338</v>
-      </c>
       <c r="S8" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="V8" s="12">
         <v>3</v>
       </c>
       <c r="Z8" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AB8" s="12">
         <v>2017</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:30" s="6" customFormat="1" ht="17">
@@ -5080,7 +5824,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D9" s="6">
         <v>42811272</v>
@@ -5089,70 +5833,70 @@
         <v>47002161</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>238</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O9" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="P9" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="P9" s="12" t="s">
-        <v>342</v>
-      </c>
       <c r="Q9" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="V9" s="6">
         <v>7</v>
       </c>
       <c r="W9" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y9" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z9" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AA9" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AB9" s="6">
         <v>2011</v>
@@ -5161,7 +5905,7 @@
         <v>22118103</v>
       </c>
       <c r="AD9" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:30" s="6" customFormat="1" ht="34">
@@ -5181,64 +5925,64 @@
         <v>10840892</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G10" s="12" t="s">
+        <v>403</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>404</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>402</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>405</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>242</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="P10" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q10" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="Q10" s="12" t="s">
-        <v>345</v>
-      </c>
       <c r="S10" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="T10" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="T10" s="12" t="s">
+      <c r="U10" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="U10" s="12" t="s">
-        <v>268</v>
       </c>
       <c r="V10" s="12">
         <v>19</v>
       </c>
       <c r="W10" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="X10" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="X10" s="12" t="s">
+      <c r="Y10" s="12" t="s">
         <v>347</v>
       </c>
-      <c r="Y10" s="12" t="s">
+      <c r="AA10" s="12" t="s">
         <v>348</v>
-      </c>
-      <c r="AA10" s="12" t="s">
-        <v>349</v>
       </c>
       <c r="AB10" s="12">
         <v>2016</v>
@@ -5247,7 +5991,7 @@
         <v>27225349</v>
       </c>
       <c r="AD10" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:30" s="6" customFormat="1" ht="51">
@@ -5258,7 +6002,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D11" s="6">
         <v>20346401</v>
@@ -5267,49 +6011,49 @@
         <v>20423092</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G11" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>408</v>
       </c>
-      <c r="H11" s="13" t="s">
-        <v>424</v>
-      </c>
-      <c r="I11" s="12" t="s">
+      <c r="J11" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>409</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>410</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>238</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O11" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="P11" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="P11" s="12" t="s">
+      <c r="Q11" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="Q11" s="12" t="s">
+      <c r="S11" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="S11" s="12" t="s">
+      <c r="T11" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="Z11" s="12" t="s">
         <v>355</v>
-      </c>
-      <c r="T11" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="Z11" s="12" t="s">
-        <v>356</v>
       </c>
       <c r="AB11" s="12">
         <v>2014</v>
@@ -5326,59 +6070,59 @@
         <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" t="s">
+        <v>412</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>418</v>
-      </c>
-      <c r="F12" t="s">
-        <v>413</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>419</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>243</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="R12" s="8"/>
       <c r="S12" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="T12" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U12" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="U12" s="14" t="s">
-        <v>268</v>
       </c>
       <c r="V12" s="14">
         <v>23</v>
@@ -5387,7 +6131,7 @@
       <c r="X12" s="8"/>
       <c r="Y12" s="8"/>
       <c r="Z12" s="14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AA12" s="8"/>
       <c r="AB12" s="14">
@@ -5415,64 +6159,64 @@
         <v>24056173</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G13" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>421</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>422</v>
-      </c>
       <c r="I13" s="13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>244</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O13" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="P13" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="P13" s="12" t="s">
+      <c r="Q13" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="Q13" s="12" t="s">
-        <v>360</v>
-      </c>
       <c r="S13" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T13" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="U13" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="U13" s="12" t="s">
-        <v>268</v>
       </c>
       <c r="V13" s="12">
         <v>13</v>
       </c>
       <c r="W13" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="X13" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="X13" s="12" t="s">
+      <c r="Y13" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="Y13" s="12" t="s">
+      <c r="AA13" s="12" t="s">
         <v>363</v>
-      </c>
-      <c r="AA13" s="12" t="s">
-        <v>364</v>
       </c>
       <c r="AB13" s="12">
         <v>2016</v>
@@ -5481,7 +6225,7 @@
         <v>26923438</v>
       </c>
       <c r="AD13" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:30" s="6" customFormat="1" ht="34">
@@ -5492,7 +6236,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D14" s="6">
         <v>103500611</v>
@@ -5501,52 +6245,52 @@
         <v>103662790</v>
       </c>
       <c r="F14" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>435</v>
-      </c>
       <c r="H14" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>439</v>
-      </c>
       <c r="J14" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>245</v>
       </c>
       <c r="M14" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="P14" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="N14" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="O14" s="6" t="s">
+      <c r="Q14" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="X14" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="P14" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>430</v>
-      </c>
-      <c r="S14" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="T14" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="X14" s="6" t="s">
+      <c r="Y14" s="6" t="s">
         <v>432</v>
-      </c>
-      <c r="Y14" s="6" t="s">
-        <v>433</v>
       </c>
       <c r="AB14" s="6">
         <v>2014</v>
@@ -5555,75 +6299,2495 @@
         <v>24733244</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+    <row r="15" spans="1:30" ht="34">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6">
+        <v>144770078</v>
+      </c>
+      <c r="D15" s="6">
+        <v>44759527</v>
+      </c>
+      <c r="E15" s="6">
+        <v>144789479</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>463</v>
+      </c>
       <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
+      <c r="K15" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>455</v>
+      </c>
       <c r="R15" s="8"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="8"/>
+      <c r="S15" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="T15" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U15" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V15" s="14">
+        <v>1</v>
+      </c>
+      <c r="W15" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="X15" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="Y15" s="14" t="s">
+        <v>458</v>
+      </c>
       <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="8"/>
+      <c r="AA15" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="AB15" s="14">
+        <v>1992</v>
+      </c>
+      <c r="AC15" s="14">
+        <v>1384046</v>
+      </c>
+      <c r="AD15" s="16" t="s">
+        <v>307</v>
+      </c>
     </row>
-    <row r="16" spans="1:30">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+    <row r="16" spans="1:30" ht="34">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3</v>
+      </c>
+      <c r="C16" s="6">
+        <v>43261945</v>
+      </c>
+      <c r="D16" s="6">
+        <v>43249864</v>
+      </c>
+      <c r="E16" s="6">
+        <v>43294691</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="G16" t="s">
+        <v>472</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>475</v>
+      </c>
       <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="6"/>
+      <c r="K16" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="L16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>467</v>
+      </c>
+      <c r="R16" s="8"/>
+      <c r="S16" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="T16" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U16" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V16" s="14">
+        <v>3</v>
+      </c>
+      <c r="W16" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="X16" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="Y16" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB16" s="14">
+        <v>2006</v>
+      </c>
+      <c r="AC16" s="14">
+        <v>16344554</v>
+      </c>
+      <c r="AD16" s="16" t="s">
+        <v>307</v>
+      </c>
     </row>
-    <row r="20" spans="2:9">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+    <row r="17" spans="1:30">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6">
+        <v>21</v>
+      </c>
+      <c r="C17" s="6">
+        <v>69352995</v>
+      </c>
+      <c r="D17" s="6">
+        <v>69348993</v>
+      </c>
+      <c r="E17" s="6">
+        <v>69356401</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="G17" t="s">
+        <v>485</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>478</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q17" s="14" t="s">
+        <v>480</v>
+      </c>
+      <c r="R17" s="8"/>
+      <c r="S17" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="T17" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U17" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V17" s="14">
+        <v>21</v>
+      </c>
+      <c r="W17" s="14" t="s">
+        <v>481</v>
+      </c>
+      <c r="X17" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="Y17" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="AB17" s="14">
+        <v>2014</v>
+      </c>
+      <c r="AC17" s="14">
+        <v>25052073</v>
+      </c>
+      <c r="AD17" s="14" t="s">
+        <v>298</v>
+      </c>
     </row>
-    <row r="26" spans="2:9">
-      <c r="I26" s="6"/>
+    <row r="18" spans="1:30">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D18" s="6">
+        <v>76789248</v>
+      </c>
+      <c r="E18" s="6">
+        <v>76840637</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="G18" t="s">
+        <v>498</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="L18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>487</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O18" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P18" s="14" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q18" s="14" t="s">
+        <v>490</v>
+      </c>
+      <c r="R18" s="8"/>
+      <c r="S18" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="T18" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U18" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="V18" s="14">
+        <v>15</v>
+      </c>
+      <c r="W18" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="X18" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="Y18" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="14">
+        <v>2006</v>
+      </c>
+      <c r="AC18" s="14">
+        <v>16859890</v>
+      </c>
+      <c r="AD18" s="14" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6">
+        <v>21</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6">
+        <v>20722980</v>
+      </c>
+      <c r="E19" s="6">
+        <v>20787646</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="G19" t="s">
+        <v>509</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="L19" t="s">
+        <v>48</v>
+      </c>
+      <c r="M19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q19" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="R19" s="8"/>
+      <c r="S19" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="T19" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U19" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V19" s="14">
+        <v>21</v>
+      </c>
+      <c r="W19" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="X19" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y19" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="14">
+        <v>2012</v>
+      </c>
+      <c r="AC19" s="14">
+        <v>22952632</v>
+      </c>
+      <c r="AD19" s="16" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6">
+        <v>69127863</v>
+      </c>
+      <c r="E20" s="6">
+        <v>69178521</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="G20" t="s">
+        <v>520</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="L20" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" t="s">
+        <v>49</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="P20" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q20" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="R20" s="8"/>
+      <c r="S20" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="T20" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U20" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V20" s="14">
+        <v>1</v>
+      </c>
+      <c r="W20" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="X20" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="Y20" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="14">
+        <v>1993</v>
+      </c>
+      <c r="AC20" s="14">
+        <v>8486364</v>
+      </c>
+      <c r="AD20" s="16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="34">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="6">
+        <v>27</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D21" s="6">
+        <v>16293899</v>
+      </c>
+      <c r="E21" s="6">
+        <v>16313546</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="G21" t="s">
+        <v>542</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="L21" t="s">
+        <v>59</v>
+      </c>
+      <c r="M21" t="s">
+        <v>451</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="U21" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="V21" s="6">
+        <v>27</v>
+      </c>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="18" t="s">
+        <v>539</v>
+      </c>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6">
+        <v>2004</v>
+      </c>
+      <c r="AC21" s="6">
+        <v>15566468</v>
+      </c>
+      <c r="AD21" s="16" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="6">
+        <v>11</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D22" s="6">
+        <v>100770166</v>
+      </c>
+      <c r="E22" s="6">
+        <v>100822252</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="G22" t="s">
+        <v>531</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="L22" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" t="s">
+        <v>61</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="P22" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q22" s="14" t="s">
+        <v>526</v>
+      </c>
+      <c r="R22" s="8"/>
+      <c r="S22" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="T22" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U22" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V22" s="14">
+        <v>11</v>
+      </c>
+      <c r="W22" s="14" t="s">
+        <v>527</v>
+      </c>
+      <c r="X22" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="Y22" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="14">
+        <v>1989</v>
+      </c>
+      <c r="AC22" s="14">
+        <v>2813370</v>
+      </c>
+      <c r="AD22" s="16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="6">
+        <v>11</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="D23" s="6">
+        <v>77885935</v>
+      </c>
+      <c r="E23" s="6">
+        <v>77927967</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="G23" t="s">
+        <v>548</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="L23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" t="s">
+        <v>66</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q23" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="R23" s="8"/>
+      <c r="S23" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="14" t="s">
+        <v>545</v>
+      </c>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="14">
+        <v>2016</v>
+      </c>
+      <c r="AC23" s="14">
+        <v>26763170</v>
+      </c>
+      <c r="AD23" s="8"/>
+    </row>
+    <row r="24" spans="1:30">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="G24" t="s">
+        <v>317</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="L24" t="s">
+        <v>76</v>
+      </c>
+      <c r="M24" t="s">
+        <v>71</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="V24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="W24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="X24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AA24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AC24" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD24" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="6">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>62810245</v>
+      </c>
+      <c r="D25" s="6">
+        <v>62784906</v>
+      </c>
+      <c r="E25" s="6">
+        <v>62888247</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="G25" t="s">
+        <v>559</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="L25" t="s">
+        <v>54</v>
+      </c>
+      <c r="M25" t="s">
+        <v>84</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O25" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="P25" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="Q25" s="14" t="s">
+        <v>553</v>
+      </c>
+      <c r="R25" s="8"/>
+      <c r="S25" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="T25" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U25" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V25" s="14">
+        <v>5</v>
+      </c>
+      <c r="W25" s="14" t="s">
+        <v>554</v>
+      </c>
+      <c r="X25" s="14" t="s">
+        <v>555</v>
+      </c>
+      <c r="Y25" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB25" s="14">
+        <v>2016</v>
+      </c>
+      <c r="AC25" s="14">
+        <v>27289157</v>
+      </c>
+      <c r="AD25" s="16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="G26" t="s">
+        <v>309</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="L26" t="s">
+        <v>54</v>
+      </c>
+      <c r="M26" t="s">
+        <v>89</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="S26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="T26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="U26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="V26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="W26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="X26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AA26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AC26" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD26" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="6">
+        <v>8</v>
+      </c>
+      <c r="C27" s="6">
+        <v>93753358</v>
+      </c>
+      <c r="D27" s="6">
+        <v>93707084</v>
+      </c>
+      <c r="E27" s="6">
+        <v>93754793</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="G27" t="s">
+        <v>574</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="L27" t="s">
+        <v>54</v>
+      </c>
+      <c r="M27" t="s">
+        <v>94</v>
+      </c>
+      <c r="N27" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O27" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="P27" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="Q27" s="14" t="s">
+        <v>567</v>
+      </c>
+      <c r="R27" s="8"/>
+      <c r="S27" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="T27" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U27" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V27" s="14">
+        <v>8</v>
+      </c>
+      <c r="W27" s="14" t="s">
+        <v>568</v>
+      </c>
+      <c r="X27" s="14" t="s">
+        <v>569</v>
+      </c>
+      <c r="Y27" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="14" t="s">
+        <v>571</v>
+      </c>
+      <c r="AB27" s="14">
+        <v>2014</v>
+      </c>
+      <c r="AC27" s="14">
+        <v>24667746</v>
+      </c>
+      <c r="AD27" s="16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="6">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1997582</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1985522</v>
+      </c>
+      <c r="E28" s="6">
+        <v>2012383</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="G28" t="s">
+        <v>584</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6" t="s">
+        <v>585</v>
+      </c>
+      <c r="L28" t="s">
+        <v>54</v>
+      </c>
+      <c r="M28" t="s">
+        <v>99</v>
+      </c>
+      <c r="N28" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P28" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="Q28" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="R28" s="8"/>
+      <c r="S28" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="T28" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U28" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V28" s="14">
+        <v>1</v>
+      </c>
+      <c r="W28" s="14" t="s">
+        <v>579</v>
+      </c>
+      <c r="X28" s="14" t="s">
+        <v>580</v>
+      </c>
+      <c r="Y28" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="Z28" s="8"/>
+      <c r="AA28" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="AB28" s="14">
+        <v>2013</v>
+      </c>
+      <c r="AC28" s="14">
+        <v>23762392</v>
+      </c>
+      <c r="AD28" s="16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="6">
+        <v>9</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6">
+        <v>91865619</v>
+      </c>
+      <c r="E29" s="6">
+        <v>91932590</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>590</v>
+      </c>
+      <c r="G29" t="s">
+        <v>591</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="L29" t="s">
+        <v>54</v>
+      </c>
+      <c r="M29" t="s">
+        <v>104</v>
+      </c>
+      <c r="N29" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O29" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P29" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="Q29" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="R29" s="8"/>
+      <c r="S29" s="14" t="s">
+        <v>588</v>
+      </c>
+      <c r="T29" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
+      <c r="Z29" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="AA29" s="8"/>
+      <c r="AB29" s="14">
+        <v>2016</v>
+      </c>
+      <c r="AC29" s="14">
+        <v>27128314</v>
+      </c>
+      <c r="AD29" s="8"/>
+    </row>
+    <row r="30" spans="1:30">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="6">
+        <v>16</v>
+      </c>
+      <c r="C30" s="6">
+        <v>29020700</v>
+      </c>
+      <c r="D30" s="6">
+        <v>29005214</v>
+      </c>
+      <c r="E30" s="6">
+        <v>29020714</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="G30" t="s">
+        <v>600</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="L30" t="s">
+        <v>54</v>
+      </c>
+      <c r="M30" t="s">
+        <v>109</v>
+      </c>
+      <c r="N30" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O30" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P30" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="Q30" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="R30" s="8"/>
+      <c r="S30" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="T30" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U30" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V30" s="14">
+        <v>16</v>
+      </c>
+      <c r="W30" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+      <c r="Z30" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="AA30" s="14" t="s">
+        <v>598</v>
+      </c>
+      <c r="AB30" s="14">
+        <v>2018</v>
+      </c>
+      <c r="AC30" s="14">
+        <v>29680649</v>
+      </c>
+      <c r="AD30" s="8"/>
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="6">
+        <v>27</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D31" s="6">
+        <v>15119556</v>
+      </c>
+      <c r="E31" s="6">
+        <v>15165355</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="G31" t="s">
+        <v>609</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="L31" t="s">
+        <v>54</v>
+      </c>
+      <c r="M31" t="s">
+        <v>114</v>
+      </c>
+      <c r="N31" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O31" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P31" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q31" s="14" t="s">
+        <v>605</v>
+      </c>
+      <c r="R31" s="8"/>
+      <c r="S31" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="T31" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U31" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V31" s="14">
+        <v>27</v>
+      </c>
+      <c r="W31" s="14" t="s">
+        <v>606</v>
+      </c>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8"/>
+      <c r="Z31" s="14" t="s">
+        <v>607</v>
+      </c>
+      <c r="AA31" s="8"/>
+      <c r="AB31" s="14">
+        <v>2020</v>
+      </c>
+      <c r="AC31" s="14">
+        <v>31733857</v>
+      </c>
+      <c r="AD31" s="8"/>
+    </row>
+    <row r="32" spans="1:30">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="6">
+        <v>5</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="D32" s="6">
+        <v>32283180</v>
+      </c>
+      <c r="E32" s="6">
+        <v>32313172</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>639</v>
+      </c>
+      <c r="G32" t="s">
+        <v>640</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" t="s">
+        <v>48</v>
+      </c>
+      <c r="M32" t="s">
+        <v>119</v>
+      </c>
+      <c r="N32" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O32" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P32" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q32" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="R32" s="8"/>
+      <c r="S32" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="T32" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U32" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="V32" s="14">
+        <v>5</v>
+      </c>
+      <c r="W32" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="8"/>
+      <c r="Z32" s="14" t="s">
+        <v>616</v>
+      </c>
+      <c r="AA32" s="8"/>
+      <c r="AB32" s="14">
+        <v>2020</v>
+      </c>
+      <c r="AC32" s="14">
+        <v>33316082</v>
+      </c>
+      <c r="AD32" s="8"/>
+    </row>
+    <row r="33" spans="1:30">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="6">
+        <v>5</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="D33" s="6">
+        <v>32283180</v>
+      </c>
+      <c r="E33" s="6">
+        <v>32313172</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>639</v>
+      </c>
+      <c r="G33" t="s">
+        <v>640</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" t="s">
+        <v>48</v>
+      </c>
+      <c r="M33" t="s">
+        <v>119</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q33" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="R33" s="8"/>
+      <c r="S33" s="14" t="s">
+        <v>617</v>
+      </c>
+      <c r="T33" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U33" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="V33" s="14">
+        <v>5</v>
+      </c>
+      <c r="W33" s="14" t="s">
+        <v>618</v>
+      </c>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="8"/>
+      <c r="Z33" s="8"/>
+      <c r="AA33" s="8"/>
+      <c r="AB33" s="14">
+        <v>2020</v>
+      </c>
+      <c r="AC33" s="14">
+        <v>32894162</v>
+      </c>
+      <c r="AD33" s="8"/>
+    </row>
+    <row r="34" spans="1:30">
+      <c r="A34" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6">
+        <v>32283180</v>
+      </c>
+      <c r="E34" s="6">
+        <v>32313172</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="G34" t="s">
+        <v>640</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" t="s">
+        <v>48</v>
+      </c>
+      <c r="M34" t="s">
+        <v>119</v>
+      </c>
+      <c r="N34" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O34" s="14" t="s">
+        <v>619</v>
+      </c>
+      <c r="P34" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q34" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="R34" s="8"/>
+      <c r="S34" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="T34" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U34" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V34" s="14">
+        <v>5</v>
+      </c>
+      <c r="W34" s="14" t="s">
+        <v>620</v>
+      </c>
+      <c r="X34" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="Y34" s="14" t="s">
+        <v>622</v>
+      </c>
+      <c r="Z34" s="8"/>
+      <c r="AA34" s="8"/>
+      <c r="AB34" s="14">
+        <v>2017</v>
+      </c>
+      <c r="AC34" s="14">
+        <v>28904385</v>
+      </c>
+      <c r="AD34" s="14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30">
+      <c r="A35" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6">
+        <v>32283180</v>
+      </c>
+      <c r="E35" s="6">
+        <v>32313172</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="G35" t="s">
+        <v>640</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M35" t="s">
+        <v>119</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="P35" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q35" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="T35" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="U35" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="V35" s="6">
+        <v>5</v>
+      </c>
+      <c r="W35" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="X35" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="Y35" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="6"/>
+      <c r="AB35" s="6">
+        <v>2017</v>
+      </c>
+      <c r="AC35" s="6">
+        <v>28904385</v>
+      </c>
+      <c r="AD35" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30">
+      <c r="A36" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6">
+        <v>32283180</v>
+      </c>
+      <c r="E36" s="6">
+        <v>32313172</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="G36" t="s">
+        <v>640</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" t="s">
+        <v>48</v>
+      </c>
+      <c r="M36" t="s">
+        <v>119</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="P36" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="T36" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="U36" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="V36" s="6">
+        <v>5</v>
+      </c>
+      <c r="W36" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="X36" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="Y36" s="6"/>
+      <c r="Z36" s="6"/>
+      <c r="AA36" s="6"/>
+      <c r="AB36" s="6">
+        <v>2016</v>
+      </c>
+      <c r="AC36" s="6">
+        <v>27296271</v>
+      </c>
+      <c r="AD36" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30">
+      <c r="A37" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6">
+        <v>32283180</v>
+      </c>
+      <c r="E37" s="6">
+        <v>32313172</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="G37" t="s">
+        <v>640</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" t="s">
+        <v>48</v>
+      </c>
+      <c r="M37" t="s">
+        <v>119</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="T37" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="U37" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="V37" s="6">
+        <v>5</v>
+      </c>
+      <c r="W37" s="6" t="s">
+        <v>630</v>
+      </c>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="Z37" s="6"/>
+      <c r="AA37" s="6"/>
+      <c r="AB37" s="6">
+        <v>2014</v>
+      </c>
+      <c r="AC37" s="6">
+        <v>25017103</v>
+      </c>
+      <c r="AD37" s="6"/>
+    </row>
+    <row r="38" spans="1:30">
+      <c r="A38" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="B38" s="6">
+        <v>5</v>
+      </c>
+      <c r="C38" s="6">
+        <v>32308008</v>
+      </c>
+      <c r="D38" s="6">
+        <v>32283180</v>
+      </c>
+      <c r="E38" s="6">
+        <v>32313172</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="G38" t="s">
+        <v>640</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" t="s">
+        <v>48</v>
+      </c>
+      <c r="M38" t="s">
+        <v>119</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q38" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="T38" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="U38" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="V38" s="6">
+        <v>5</v>
+      </c>
+      <c r="W38" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="X38" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="Y38" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="Z38" s="6"/>
+      <c r="AA38" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="AB38" s="6">
+        <v>2017</v>
+      </c>
+      <c r="AC38" s="6">
+        <v>28904385</v>
+      </c>
+      <c r="AD38" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30">
+      <c r="A39" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6">
+        <v>32283180</v>
+      </c>
+      <c r="E39" s="6">
+        <v>32313172</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="G39" t="s">
+        <v>640</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" t="s">
+        <v>48</v>
+      </c>
+      <c r="M39" t="s">
+        <v>119</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="T39" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="U39" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="V39" s="6">
+        <v>5</v>
+      </c>
+      <c r="W39" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="X39" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="Y39" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="Z39" s="6"/>
+      <c r="AA39" s="6"/>
+      <c r="AB39" s="6">
+        <v>2019</v>
+      </c>
+      <c r="AC39" s="6">
+        <v>30378686</v>
+      </c>
+      <c r="AD39" s="6"/>
+    </row>
+    <row r="40" spans="1:30">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G40" t="s">
+        <v>309</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="N40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="P40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="R40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="T40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="U40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="V40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="W40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="X40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AA40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AC40" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD40" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="6">
+        <v>3</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6">
+        <v>9350633</v>
+      </c>
+      <c r="E41" s="6">
+        <v>9394688</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="N41" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O41" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="P41" s="14" t="s">
+        <v>646</v>
+      </c>
+      <c r="Q41" s="14" t="s">
+        <v>647</v>
+      </c>
+      <c r="R41" s="14" t="s">
+        <v>648</v>
+      </c>
+      <c r="S41" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="T41" s="14" t="s">
+        <v>649</v>
+      </c>
+      <c r="U41" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V41" s="14">
+        <v>3</v>
+      </c>
+      <c r="W41" s="14" t="s">
+        <v>650</v>
+      </c>
+      <c r="X41" s="14" t="s">
+        <v>651</v>
+      </c>
+      <c r="Y41" s="14" t="s">
+        <v>652</v>
+      </c>
+      <c r="Z41" s="8"/>
+      <c r="AA41" s="8"/>
+      <c r="AB41" s="14">
+        <v>2017</v>
+      </c>
+      <c r="AC41" s="14">
+        <v>28904385</v>
+      </c>
+      <c r="AD41" s="14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30">
+      <c r="A42" t="s">
+        <v>654</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="G42" t="s">
+        <v>309</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="L42" t="s">
+        <v>212</v>
+      </c>
+      <c r="M42" t="s">
+        <v>655</v>
+      </c>
+      <c r="N42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="P42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="R42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="S42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="T42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="U42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="V42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="W42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="X42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AA42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AC42" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD42" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30">
+      <c r="A43" t="s">
+        <v>654</v>
+      </c>
+      <c r="B43" s="6">
+        <v>15</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6">
+        <v>15447722</v>
+      </c>
+      <c r="E43" s="6">
+        <v>15456214</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="G43" t="s">
+        <v>666</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>667</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>668</v>
+      </c>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="L43" t="s">
+        <v>54</v>
+      </c>
+      <c r="M43" t="s">
+        <v>656</v>
+      </c>
+      <c r="N43" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="O43" s="14" t="s">
+        <v>659</v>
+      </c>
+      <c r="P43" s="14" t="s">
+        <v>660</v>
+      </c>
+      <c r="Q43" s="14" t="s">
+        <v>661</v>
+      </c>
+      <c r="R43" s="8"/>
+      <c r="S43" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="T43" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="U43" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="V43" s="14">
+        <v>15</v>
+      </c>
+      <c r="W43" s="14" t="s">
+        <v>662</v>
+      </c>
+      <c r="X43" s="14" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y43" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="Z43" s="8"/>
+      <c r="AA43" s="8"/>
+      <c r="AB43" s="14">
+        <v>2013</v>
+      </c>
+      <c r="AC43" s="14">
+        <v>23349982</v>
+      </c>
+      <c r="AD43" s="16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30">
+      <c r="A44" t="s">
+        <v>654</v>
+      </c>
+      <c r="B44" s="6">
+        <v>26</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>670</v>
+      </c>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
+        <v>671</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>309</v>
+      </c>
+      <c r="H44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="I44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="J44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="K44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="L44" t="s">
+        <v>54</v>
+      </c>
+      <c r="M44" t="s">
+        <v>657</v>
+      </c>
+      <c r="N44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="O44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="P44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="R44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="S44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="T44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="U44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="V44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="W44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="X44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="AA44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="AC44" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD44" s="29" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
+      <c r="U45" s="6"/>
+      <c r="V45" s="6"/>
+      <c r="W45" s="6"/>
+      <c r="X45" s="6"/>
+      <c r="Y45" s="6"/>
+      <c r="Z45" s="6"/>
+      <c r="AA45" s="6"/>
+      <c r="AB45" s="6"/>
+      <c r="AC45" s="6"/>
+      <c r="AD45" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -5632,11 +8796,21 @@
     <hyperlink ref="AD7" r:id="rId2" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{B60A99FD-0C8B-EC4B-A9FA-00FD4C228C68}"/>
     <hyperlink ref="AD10" r:id="rId3" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{0F14DC3C-6185-1C4E-9471-581DD7F01AAD}"/>
     <hyperlink ref="AD13" r:id="rId4" display="https://doi.org/10.1186/1471-2164-14-446" xr:uid="{10561EFE-5896-9F41-A883-2CDD80893631}"/>
+    <hyperlink ref="AD15" r:id="rId5" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{7CF4169B-51BE-AC4B-99D6-70D044756105}"/>
+    <hyperlink ref="AD16" r:id="rId6" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{A10A0C06-EEB9-384B-8844-31D5D4D75C52}"/>
+    <hyperlink ref="AD19" r:id="rId7" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{2BC2EEE8-E34D-E84B-AD96-8793F79212E8}"/>
+    <hyperlink ref="AD20" r:id="rId8" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{56DA6B2E-5048-B041-982F-1B18C920595B}"/>
+    <hyperlink ref="AD22" r:id="rId9" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{5C827C09-A22A-C34B-BB09-5CE34DF1DD68}"/>
+    <hyperlink ref="AD21" r:id="rId10" xr:uid="{2CAEC663-1644-E64B-8F8A-0602D5BBB954}"/>
+    <hyperlink ref="AD25" r:id="rId11" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{015CA8FC-A4E2-D243-A632-E81EB10B8F4B}"/>
+    <hyperlink ref="AD27" r:id="rId12" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{78B2A735-F61E-374F-82E8-38F87079A9FD}"/>
+    <hyperlink ref="AD28" r:id="rId13" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{BD9CB8EC-D2B9-4749-9470-05196DBBB2DC}"/>
+    <hyperlink ref="AD43" r:id="rId14" display="https://www.icbf.com/wp/?page_id=2170" xr:uid="{6B7BDEB9-1797-5C4C-A098-18A374FC2D1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5645,8 +8819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B96105-ED37-6A48-B14A-8CDBB38B2477}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5655,10 +8829,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5675,24 +8849,24 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23" t="s">
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="23" t="s">
+      <c r="J2" s="27"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="25"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="1:13" ht="34">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
Adding Polled horns trait
</commit_message>
<xml_diff>
--- a/SVs_identification/results/Summary of monogenous traits.xlsx
+++ b/SVs_identification/results/Summary of monogenous traits.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/breedmaps/SVs_identification/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jenny/breedmaps/SVs_identification/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14D2EAB-7830-474E-BF0F-8F0D696195AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B86B07-45D7-FA46-9E31-3698BB8C6350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12220" yWindow="500" windowWidth="16580" windowHeight="16380" xr2:uid="{000CD8DE-5782-4E40-B73D-11CA3F163355}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="27320" windowHeight="13700" xr2:uid="{000CD8DE-5782-4E40-B73D-11CA3F163355}"/>
   </bookViews>
   <sheets>
     <sheet name="All info" sheetId="2" r:id="rId1"/>
-    <sheet name="Traits" sheetId="1" r:id="rId2"/>
+    <sheet name="Blad1" sheetId="3" r:id="rId2"/>
+    <sheet name="Traits" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="variants" localSheetId="1">Blad1!$A$1:$R$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,8 +38,37 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{58530A8E-855A-3F4D-B80E-8DDF849B88B7}" name="variants" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/Jenny/Downloads/variants.csv" decimal="," thousands=" " tab="0" delimiter=",">
+      <textFields count="18">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="711">
   <si>
     <r>
       <rPr>
@@ -3963,6 +3996,124 @@
   </si>
   <si>
     <t>OMIA001942-9913</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>OMIA ID(s)</t>
+  </si>
+  <si>
+    <t>OMIA 000483-9913</t>
+  </si>
+  <si>
+    <t>Nellore</t>
+  </si>
+  <si>
+    <t>Polled, Guarani</t>
+  </si>
+  <si>
+    <t>POLLED</t>
+  </si>
+  <si>
+    <t>P[sub]G</t>
+  </si>
+  <si>
+    <t>duplication</t>
+  </si>
+  <si>
+    <t>g.2614828_2724315dup</t>
+  </si>
+  <si>
+    <t>"a novel duplication variant" in the region BTA1:1,893,790‚Äì2,004,553 (Utsunomiya et al., (2019)</t>
+  </si>
+  <si>
+    <t>Randhawa et al. (2019): ARS-UCD1.2 g.2614828_2724315dup</t>
+  </si>
+  <si>
+    <t>Friesian</t>
+  </si>
+  <si>
+    <t>Polled, Friesian</t>
+  </si>
+  <si>
+    <t>P[sub]F OR¬†P(sub)80kbID</t>
+  </si>
+  <si>
+    <t>g.2629113_2709240dup</t>
+  </si>
+  <si>
+    <t>In relation to assembly UMD v3.1.1, Utsunomiya et al. (2019) described this variant as "a duplication of CHR1:1,909,352‚Äì1,989,480".</t>
+  </si>
+  <si>
+    <t>Randhawa et al. (2019): ARS-UCD1.2  g.2629113_2709240dup"</t>
+  </si>
+  <si>
+    <t>Brahman</t>
+  </si>
+  <si>
+    <t>Polled, Celtic</t>
+  </si>
+  <si>
+    <t>P[sub]C OR P[sub]202ID</t>
+  </si>
+  <si>
+    <t>g.[22429326_2429335del;2429109_2429320dupins]</t>
+  </si>
+  <si>
+    <t>UMD3.1: g.1706051_1706060 delins170583</t>
+  </si>
+  <si>
+    <t>Randhawa et al. (2019) ARS-UCD1.2 g.[22429326_2429335del;2429109_2429320dupins]</t>
+  </si>
+  <si>
+    <t>Mongolian Turano</t>
+  </si>
+  <si>
+    <t>Polled, Mongolian</t>
+  </si>
+  <si>
+    <t>P[sub]M OR P[sub]219ID</t>
+  </si>
+  <si>
+    <t>g.[2695261_2695267delinsTCTGAA;2695889_2696047dupins]</t>
+  </si>
+  <si>
+    <t>"a complex 219-bp duplication-insertion (P219ID) beginning at 1,976,128 bp and a 7-bp deletion and 6-bp insertion (P1ID) located 621 bp upstream of this position . . . . This rearrangement results in duplication of an 11-bp motif (5'-AAAGAAGCAAA-3') that is entirely conserved among Bovidae . . . and that is also duplicated in the 80-kb duplication responsible for Friesian polledness"</t>
+  </si>
+  <si>
+    <t>In relation to assembly UMD v3.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Utsunomiya et al. (2019) described this variant as ""a complex duplication starting at CHR1:1</t>
+  </si>
+  <si>
+    <t>128""."</t>
+  </si>
+  <si>
+    <t>Randhawa et al. (2019): ARS-UCD1.2 g.[2695261_2695267delinsTCTGAA;2695889_2696047dupins]</t>
+  </si>
+  <si>
+    <t>Randhawa et al. (2019): ARS-UCD1.2 g.2614828_2724315dup
+Randhawa et al. (2019): ARS-UCD1.2  g.2629113_2709240dup"</t>
+  </si>
+  <si>
+    <t>2614828-2724315</t>
+  </si>
+  <si>
+    <t>2629113-2709240</t>
+  </si>
+  <si>
+    <t>2695261-2695267;2695889-2696047</t>
+  </si>
+  <si>
+    <t>22429326-2429335;2429109-2429320</t>
+  </si>
+  <si>
+    <t>125 CNVs in total</t>
+  </si>
+  <si>
+    <t>Very many SVs</t>
   </si>
 </sst>
 </file>
@@ -4145,7 +4296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4181,6 +4332,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4211,8 +4364,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -4782,9 +4936,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="variants" connectionId="1" xr16:uid="{5558F8FC-3205-FD44-A291-7C838DFF38DC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53E3D7F1-38C9-AB46-99BA-209E7F03E84D}" name="Tabell1" displayName="Tabell1" ref="A1:AD45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A1:AD45" xr:uid="{0AA2673E-FE49-C747-96B4-3C5666F9D2F9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53E3D7F1-38C9-AB46-99BA-209E7F03E84D}" name="Tabell1" displayName="Tabell1" ref="A1:AD48" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A1:AD48" xr:uid="{0AA2673E-FE49-C747-96B4-3C5666F9D2F9}"/>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{ACE7D78E-E96B-1F4D-8067-F66CD3F7FD27}" name="BREED-VEXA" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{085AC52D-1D2E-754A-A01E-C239BDEE8C5D}" name="Chr" dataDxfId="27"/>
@@ -5118,10 +5276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5724AFB8-EF24-374C-BA51-A6E5C12EB880}">
-  <dimension ref="A1:AD45"/>
+  <dimension ref="A1:AD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8677,27 +8835,27 @@
       <c r="B44" s="6">
         <v>26</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="19" t="s">
         <v>670</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29" t="s">
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19" t="s">
         <v>671</v>
       </c>
-      <c r="G44" s="30" t="s">
-        <v>309</v>
-      </c>
-      <c r="H44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="I44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="J44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="K44" s="29" t="s">
+      <c r="G44" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="J44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="K44" s="19" t="s">
         <v>309</v>
       </c>
       <c r="L44" t="s">
@@ -8706,88 +8864,350 @@
       <c r="M44" t="s">
         <v>657</v>
       </c>
-      <c r="N44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="O44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="P44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="R44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="S44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="T44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="U44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="V44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="W44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="X44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="Y44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="Z44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="AA44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="AB44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="AC44" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="AD44" s="29" t="s">
+      <c r="N44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="O44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="P44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="R44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="S44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="T44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="U44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="V44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="W44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="X44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="AA44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="AC44" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD44" s="19" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="45" spans="1:30">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
+    <row r="45" spans="1:30" ht="34">
+      <c r="A45" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>705</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>674</v>
+      </c>
+      <c r="G45" t="s">
+        <v>309</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>710</v>
+      </c>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="6"/>
-      <c r="T45" s="6"/>
-      <c r="U45" s="6"/>
-      <c r="V45" s="6"/>
-      <c r="W45" s="6"/>
-      <c r="X45" s="6"/>
-      <c r="Y45" s="6"/>
-      <c r="Z45" s="6"/>
-      <c r="AA45" s="6"/>
-      <c r="AB45" s="6"/>
-      <c r="AC45" s="6"/>
-      <c r="AD45" s="6"/>
+      <c r="N45" t="s">
+        <v>261</v>
+      </c>
+      <c r="O45" t="s">
+        <v>675</v>
+      </c>
+      <c r="P45" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>677</v>
+      </c>
+      <c r="R45" t="s">
+        <v>678</v>
+      </c>
+      <c r="S45" t="s">
+        <v>679</v>
+      </c>
+      <c r="T45" t="s">
+        <v>649</v>
+      </c>
+      <c r="U45" t="s">
+        <v>492</v>
+      </c>
+      <c r="V45">
+        <v>1</v>
+      </c>
+      <c r="W45" t="s">
+        <v>680</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB45">
+        <v>2019</v>
+      </c>
+      <c r="AC45">
+        <v>30644114</v>
+      </c>
+      <c r="AD45" s="31" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30">
+      <c r="A46" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="B46" s="6">
+        <v>1</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>706</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>674</v>
+      </c>
+      <c r="G46" t="s">
+        <v>309</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>710</v>
+      </c>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>683</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q46" s="6" t="s">
+        <v>677</v>
+      </c>
+      <c r="R46" s="6" t="s">
+        <v>685</v>
+      </c>
+      <c r="S46" s="6" t="s">
+        <v>679</v>
+      </c>
+      <c r="T46" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="U46" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="V46" s="6">
+        <v>1</v>
+      </c>
+      <c r="W46" s="6" t="s">
+        <v>686</v>
+      </c>
+      <c r="X46" s="6"/>
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6"/>
+      <c r="AA46" s="6"/>
+      <c r="AB46" s="6">
+        <v>2013</v>
+      </c>
+      <c r="AC46" s="6">
+        <v>23717440</v>
+      </c>
+      <c r="AD46" s="6" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30">
+      <c r="A47" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="B47" s="6">
+        <v>1</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>674</v>
+      </c>
+      <c r="G47" t="s">
+        <v>309</v>
+      </c>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="P47" s="6" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q47" s="6" t="s">
+        <v>677</v>
+      </c>
+      <c r="R47" s="6" t="s">
+        <v>691</v>
+      </c>
+      <c r="S47" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="T47" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="U47" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="V47" s="6">
+        <v>1</v>
+      </c>
+      <c r="W47" s="6" t="s">
+        <v>692</v>
+      </c>
+      <c r="X47" s="6"/>
+      <c r="Y47" s="6"/>
+      <c r="Z47" s="6" t="s">
+        <v>693</v>
+      </c>
+      <c r="AA47" s="6"/>
+      <c r="AB47" s="6">
+        <v>2012</v>
+      </c>
+      <c r="AC47" s="6">
+        <v>22737241</v>
+      </c>
+      <c r="AD47" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30">
+      <c r="A48" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="B48" s="6">
+        <v>1</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>674</v>
+      </c>
+      <c r="G48" t="s">
+        <v>309</v>
+      </c>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O48" s="6" t="s">
+        <v>695</v>
+      </c>
+      <c r="P48" s="6" t="s">
+        <v>696</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>677</v>
+      </c>
+      <c r="R48" s="6" t="s">
+        <v>697</v>
+      </c>
+      <c r="S48" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="T48" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="U48" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="V48" s="6">
+        <v>1</v>
+      </c>
+      <c r="W48" s="6" t="s">
+        <v>698</v>
+      </c>
+      <c r="X48" s="6"/>
+      <c r="Y48" s="6"/>
+      <c r="Z48" s="6" t="s">
+        <v>699</v>
+      </c>
+      <c r="AA48" s="6"/>
+      <c r="AB48" s="6"/>
+      <c r="AC48" s="6"/>
+      <c r="AD48" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -8816,6 +9236,301 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05D80A7-0E5B-434D-9FA8-22DA9C815977}">
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="80.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H1" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
+        <v>282</v>
+      </c>
+      <c r="L1" t="s">
+        <v>283</v>
+      </c>
+      <c r="M1" t="s">
+        <v>284</v>
+      </c>
+      <c r="N1" t="s">
+        <v>285</v>
+      </c>
+      <c r="O1" t="s">
+        <v>286</v>
+      </c>
+      <c r="P1" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>288</v>
+      </c>
+      <c r="R1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>674</v>
+      </c>
+      <c r="B2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" t="s">
+        <v>675</v>
+      </c>
+      <c r="D2" t="s">
+        <v>676</v>
+      </c>
+      <c r="E2" t="s">
+        <v>677</v>
+      </c>
+      <c r="F2" t="s">
+        <v>678</v>
+      </c>
+      <c r="G2" t="s">
+        <v>679</v>
+      </c>
+      <c r="H2" t="s">
+        <v>649</v>
+      </c>
+      <c r="I2" t="s">
+        <v>492</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>680</v>
+      </c>
+      <c r="N2" t="s">
+        <v>681</v>
+      </c>
+      <c r="P2">
+        <v>2019</v>
+      </c>
+      <c r="Q2">
+        <v>30644114</v>
+      </c>
+      <c r="R2" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>674</v>
+      </c>
+      <c r="B3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" t="s">
+        <v>683</v>
+      </c>
+      <c r="D3" t="s">
+        <v>684</v>
+      </c>
+      <c r="E3" t="s">
+        <v>677</v>
+      </c>
+      <c r="F3" t="s">
+        <v>685</v>
+      </c>
+      <c r="G3" t="s">
+        <v>679</v>
+      </c>
+      <c r="H3" t="s">
+        <v>649</v>
+      </c>
+      <c r="I3" t="s">
+        <v>492</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>686</v>
+      </c>
+      <c r="P3">
+        <v>2013</v>
+      </c>
+      <c r="Q3">
+        <v>23717440</v>
+      </c>
+      <c r="R3" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>674</v>
+      </c>
+      <c r="B5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C5" t="s">
+        <v>689</v>
+      </c>
+      <c r="D5" t="s">
+        <v>690</v>
+      </c>
+      <c r="E5" t="s">
+        <v>677</v>
+      </c>
+      <c r="F5" t="s">
+        <v>691</v>
+      </c>
+      <c r="G5" t="s">
+        <v>588</v>
+      </c>
+      <c r="H5" t="s">
+        <v>649</v>
+      </c>
+      <c r="I5" t="s">
+        <v>492</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>692</v>
+      </c>
+      <c r="N5" t="s">
+        <v>693</v>
+      </c>
+      <c r="P5">
+        <v>2012</v>
+      </c>
+      <c r="Q5">
+        <v>22737241</v>
+      </c>
+      <c r="R5" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>674</v>
+      </c>
+      <c r="B6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6" t="s">
+        <v>695</v>
+      </c>
+      <c r="D6" t="s">
+        <v>696</v>
+      </c>
+      <c r="E6" t="s">
+        <v>677</v>
+      </c>
+      <c r="F6" t="s">
+        <v>697</v>
+      </c>
+      <c r="G6" t="s">
+        <v>588</v>
+      </c>
+      <c r="H6" t="s">
+        <v>649</v>
+      </c>
+      <c r="I6" t="s">
+        <v>492</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>698</v>
+      </c>
+      <c r="N6" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>700</v>
+      </c>
+      <c r="B7" t="s">
+        <v>701</v>
+      </c>
+      <c r="C7">
+        <v>976</v>
+      </c>
+      <c r="D7" t="s">
+        <v>702</v>
+      </c>
+      <c r="F7">
+        <v>2017</v>
+      </c>
+      <c r="G7">
+        <v>28135247</v>
+      </c>
+      <c r="H7" t="s">
+        <v>703</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B96105-ED37-6A48-B14A-8CDBB38B2477}">
   <dimension ref="A1:M45"/>
   <sheetViews>
@@ -8829,10 +9544,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -8849,24 +9564,24 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23" t="s">
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="26" t="s">
+      <c r="J2" s="29"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="28"/>
+      <c r="M2" s="30"/>
     </row>
     <row r="3" spans="1:13" ht="34">
       <c r="A3" s="2" t="s">

</xml_diff>